<commit_message>
Edit the main file
</commit_message>
<xml_diff>
--- a/Job Hunter/JHClientTarget.xlsx
+++ b/Job Hunter/JHClientTarget.xlsx
@@ -14,27 +14,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+  <x:si>
+    <x:t>Director of Product</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=101&amp;ao=1110586&amp;s=58&amp;guid=0000017d035136a985cc529157229a1b&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_9636ccf1&amp;cb=1636438194548&amp;jobListingId=1007338908659&amp;cpc=50CB34463567876F&amp;jrtk=3-0-1fk1l2dsdu46k801-1fk1l2dssu1au800-e704d3e164c9825e--6NYlbfkN0AOAePQAgQDSX6T10l2CdlahB9XGxXsykaMCL8scOYOLJPWT3z1EvnGXnjest1zb4NIA28Gb2SzRfl33MKrUwrINUzj2nUoXN__JKckXz7bi4x6ePtSMq74h6rPUrBsWou58xq__LzcB67uLL8RoGaFPe3qTM2EqaXhxPCWnObEjoXPpYFwH9Gcvc-SmFUkgqzPZD3Z8bBo4Ery1c2Ev2-lanouhjCXHWzRpk7S80ioueNkYvi-gCR_ZH2_Doi70YVmSCnBBJkcTq7fGCePI9zIGaleBCXPitfK5h4XqNkohGGg2J02xLpFvYspuox0FXZs7okzNdpVecpbezNKP9GvwO6HI5_1jGenI8Wq6BWWPZzC0u1NBBLJaNQZeapDygVqA5Nk0f7c7rv-ONbGi6XrXsyoHx9KvpJ2X78y9FbOy0aPZh1u9_Fi5ArBk766i1n-19WBDFL4RUfoUKHZYeCUyshBSlVrGrXW8qL6vDob_Prfua2_0O8e</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KIZEN Technologies, Inc.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Austin, TX</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Full-time</x:t>
+  </x:si>
   <x:si>
     <x:t>Expert Associate Director, Software</x:t>
   </x:si>
   <x:si>
-    <x:t>/partner/jobListing.htm?pos=101&amp;ao=1110586&amp;s=58&amp;guid=0000017d02900fa288e32d398d958234&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_7682e856&amp;cb=1636425536137&amp;jobListingId=1007355118481&amp;cpc=30018A8B5041CD72&amp;jrtk=3-0-1fk19044au230801-1fk190451hior800-ac7515175a77f4c0--6NYlbfkN0DoP8nG612n6SaIo-6cBFZ4ajKscvbmOmjTSQxsFZrL9I2eucWeLTh49xiULvC3ZXqLP20PfTxmoV8V6Uqx2Mavwfd7Ibmkq8SvUom5lH3D7p_0iIOw6OilIpYctcx8yiNkrrdzw06HVuZrxrUSoBrUIDaDUKJTsCqNASSk4UFUVm4arcO67DMjSmIhHoptvmx43pl6yWWgOvnxKND8qKrelP5GoCmQj3RhZawp-UJ3SuvyqeeF_2tmkAx5v2Yn8VWVyiVegtXVAcCdh-tOLzlacF7pSMukp-BGXG115id6r-w88022fDsZ-1dpteg_fGPAj7LcKqHtG7hvsfEFuRMl2fe2DPHWCBnUKwob_WAUcPIX-W-xMzmy3XIUEZ1mFGWUXS4rkJuSYRKjvD7IarGYQvryg7ajX3AsFRieEUsM7EBjDk9oNZDOfFtWHn4b8YqBzrUmhi4MxmvsN9kvRBOECBVN_kmPZf3tn-EJEoqnZpcgF2I06nRzjMqA21xNZyqLHOluQqFYiHN7_bBpLsY5CQNQbCA6bfKUDe53V5OqfV8j2Yosi5YDhxzjJNUwA9QFCyxgCoOqpSJmkEcNH8HEh3UC-DDDQ4RBDOKkp1ZaIZWBplzgwzpPSl4m68HRqOBGHafk7jMZphzhiFdX236BALUgTwX_nAP8z7Vv_YVRpMSQoPBmS_h0Xp-qnpXjR2ocPwmFBjdAlLOWsPE0Sbovl_zSs2zJ_tgzS6AlTxyDL-wvRIGXEJfpGVupxGf7ZBoazb2L52XL-584RUu0ujmKv91VQvUACswmXhGj9NABla1nU3y1hFXX05nRdxXl-U1RJrDhmzCu07E6yoqw7osDf_Y6WUMMm4ts05inpluYmkm7LmkknGuEbRKD90VPPxYkRh-4fLPyVVOBfPnVj7p6XiIDdcDkqSfOMOGTcktpixbvjVIh_iU1NvigtqbwmaNnkDc_ygZ-u-kmMWTNtumfGNmz-pa29_7xreWbYGixoY5vRatrVGziygjj7IoPWdui5Cv_-ZKGTTSlR2K_M1wJ</x:t>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=102&amp;ao=1110586&amp;s=58&amp;guid=0000017d035136a985cc529157229a1b&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_4ec789be&amp;cb=1636438194546&amp;jobListingId=1007355118481&amp;cpc=097AB8C29B9A33B8&amp;jrtk=3-0-1fk1l2dsdu46k801-1fk1l2dssu1au800-ac7515175a77f4c0--6NYlbfkN0DoP8nG612n6SaIo-6cBFZ4ajKscvbmOmjTSQxsFZrL9I2eucWeLTh49xiULvC3ZXqLP20PfTxmoV8V6Uqx2Mavwfd7Ibmkq8SvUom5lH3D7p_0iIOw6OilIpYctcx8yiNkrrdzw06HVuZrxrUSoBrUIDaDUKJTsCqNASSk4UFUVm4arcO67DMj6s1__FL5KKxairjH8exhEdXqA2_7FtIkCqKcV0ulK6ui9OAh3dU-cwOKqMjrJD0ycfiZIDP31Hrg8WSbX7XmNqfB_Kl6dJnq3a7gGOUTMXqjFM6fKaEwPLjszmiTcSAGtJ2vckXP31_uCdzsPTX3mY9eHIOIgrWftvrQ7jsjxap7cwc5dfuivKWoICPph3OeeybsWltPqZMCfIl6J9zNs4OYuzkWe3BRYuqA0-xkKWllwc9xeJQPohL1Jvu_B8SzAU-C92zvdwc3dAMN6k-1CIXv4GOCGjYdViDsWFM8c9g-RrtVKqs2faukh4PQKDyvWlrAU7-OZCXcCeKBwURkiDAAJjnlU8EGtHBg1HnPnNwiyJDIKmp5Et7iilGqEYraJeaCZ9_ZEcpRaKwDcVWOL7WrFobG5L5DK0fND7dca_AiP0TAf1xacrp8qp3es2eYhQGfuQy4G2dMe9U1Xvz6J7fP7Iz5lm14WBxJzw29Iz0BX1CXYpIybTscqlTuySrMHzxcOKJQ-Ezj_leBB7FmRw0fpaRZkaSn6v44LpsnNgq1j0TegBfZvQnuKqDXQTkMOS0XMxU8-y6xhXRNFEQqqbBEzmj9PI6cFaaHKyEQA4dvmdqEgaLTNJ8rrHRrYcWZZ6MSq6F3qtw9aU7Yr8MlRpYtIScDWux46C2HyiTHlICP_YiAlVCLrssWeI_j1YbFM9rTlvyxmD9RqyW9eVSderyJ3VOrw5TOvNAdKVsK78U7n1JOaGs8EeF4jc_tU8W4SR5aQWw6FuhoMkgRC5jH2kYa_NkmFT3KhEF-UQ9HWxXecxuP_lBr8DyYl8B8cIVmAJOCTXt5tPBmFM1T6BOE-XHt15hQwJ03</x:t>
   </x:si>
   <x:si>
     <x:t>Boston Consulting Group</x:t>
   </x:si>
   <x:si>
-    <x:t>Austin, TX</x:t>
-  </x:si>
-  <x:si>
     <x:t xml:space="preserve"> N/A</x:t>
   </x:si>
   <x:si>
     <x:t>Software Engineering Senior Advisor</x:t>
   </x:si>
   <x:si>
-    <x:t>/partner/jobListing.htm?pos=102&amp;ao=1110586&amp;s=58&amp;guid=0000017d02900fa288e32d398d958234&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_f9ff1086&amp;cb=1636425536137&amp;jobListingId=1007383667451&amp;cpc=90054033016EDCA3&amp;jrtk=3-0-1fk19044au230801-1fk190451hior800-9d4c55214232d9cd--6NYlbfkN0CJ4RVix5XbFvNEFGzeV6zdxykB_vlp8KSj_a_ovArNcpAUAf_1FZDHjCSGWhNpxUQMyoKTv9PM6XJueBvQ_5DfQXv_B9TQ5ZYRQ4CFNO3ggUgnV7IVmum8GxhrVOFwcxtXqXQ5sQdVkNfL_MK_SH3wf9qWbPfJnzDBPfD-S-Ev7zB7Kr5ZDZ0gpFt0U_fRDNds0V4goW4gPy6lbNzoOOswCQ3owA6vl4MaV9npEx-xC2pbOqnBZ2eXf6abfcPJVvpC5cpwBY3_DMadYVLeyMXyrprHXm16noCt6OfSKT0dDMDL8IKsugRzHtOiT80nMaeNOYyXSg41A4anzAeqe4Qc8us8XzOF3ieRAWPMG9xc46CEFgndHg_uJEca2R4WL1uC5FAl9usi8VN5izCHl41wjJGYQ7Fcn3GK3h4I4DWGGjo-2cFa9C-BiHRa3SjHjpNYMxTJIUnJdUxvvgbxCSjWAhLopYyMNlF1A0rT59kVjL68bYGis3Io5Oqxj9ancY6c4mClyW29V9WoNsE9OcOA52mnTPqzQWmIAzOwhJkEWCKU4KTTRb8V</x:t>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=103&amp;ao=1110586&amp;s=58&amp;guid=0000017d035136a985cc529157229a1b&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_18ec2cf2&amp;cb=1636438194547&amp;jobListingId=1007383667451&amp;cpc=54182D2BE672C5C2&amp;jrtk=3-0-1fk1l2dsdu46k801-1fk1l2dssu1au800-9d4c55214232d9cd--6NYlbfkN0CJ4RVix5XbFvNEFGzeV6zdxykB_vlp8KSj_a_ovArNcpAUAf_1FZDHjCSGWhNpxUQMyoKTv9PM6XJueBvQ_5DfQXv_B9TQ5ZYRQ4CFNO3ggUgnV7IVmum8GxhrVOFwcxtXqXQ5sQdVkNfL_MK_SH3wf9qWbPfJnzDBPfD-S-Ev7zB7Kr5ZDZ0gXyxHnyEanqkjmtT_c8RN83ltOp4f7jy2K0pxQ9PNyjjKZK_Nv4W36dtXutjsgVX3IONol4kSyveocCnWiWCL6phRdIT_UHFB3BzCMbX45SmHuKSA4kgFUtHvTo-ta92dTuT1Kd7yeV1NazxkfpKXXB1VohHQ0QpbXuvIrVE6USwuZcyFWuFXVzsgwtzJIFdn1zsDCTqE02fmy3gpE5ztXlWHKDzaCJzxBdnF3pH9jByAT09KbUmSDqjkiBbmgfS4_xOZsqq7gWFyRL8nSDLuM577suYarkgxS91ngALFsYxcMJJ0OrdNaLdxRpOwEbCkoGZ_hBoWpCPeYud6hYFdN4THNfz4ABdIkyPFFLug9loodopajqLyA5jbZ21Jr-GS</x:t>
   </x:si>
   <x:si>
     <x:t>DirectSourcePRO</x:t>
@@ -43,67 +55,64 @@
     <x:t xml:space="preserve"> Contract</x:t>
   </x:si>
   <x:si>
+    <x:t>Director of Engineering</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=104&amp;ao=1110586&amp;s=58&amp;guid=0000017d035136a985cc529157229a1b&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_c72844df&amp;cb=1636438194551&amp;jobListingId=1007324253730&amp;cpc=F7BD8DA794B5A532&amp;jrtk=3-0-1fk1l2dsdu46k801-1fk1l2dssu1au800-117d2c3d57339250--6NYlbfkN0CZjhvTnxks3zwjl9aG4M95ujhchPY6uJ5pIT_-TAyNWwWzAceZ7wwXdFj0kTHzfmG28fsS-5oi_K3xh9W0FUu0WxvJZZjBiTSyRSMOCQDnQCk9cELNatRbo6vOYcUSNivqRjZqrtAJUxJbp81YPjzFBR3Vy9WJpmIcNOUfzGLGKTHuc4JV4AY622YKdSv7sW87e1A4SAlaiAUCtJCux7PAUT9Zx3Gd4vTfDPtGq6WOeM5VXlwUpVrp7k8gJbZokPnmRjI6wYuvwgXsP1HRMb7ZE2_ZHTVHhRr1JZFKKt3c6XUuLbZQx5xqVfK1UUY96H8mi165CYSqVhUImv4uJ8KdItAzmQhl6SU8ForLhPs4Y6ba4LLeX8MPRqi9vDSrwthfAd0-WoKvUhG4BDFWnOVxqjgKWhFUaQt7L8iYLNKr3QzVWG5zyW4c0ug46xXPmlc%3D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Torc Robotics</x:t>
+  </x:si>
+  <x:si>
     <x:t>Manager of Authentication, Authorization and Directory Services Engineering</x:t>
   </x:si>
   <x:si>
-    <x:t>/partner/jobListing.htm?pos=103&amp;ao=1110586&amp;s=58&amp;guid=0000017d02900fa288e32d398d958234&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_cde55b27&amp;cb=1636425536140&amp;jobListingId=1007372201346&amp;cpc=88825F42635DFB7C&amp;jrtk=3-0-1fk19044au230801-1fk190451hior800-dc314448be7afab2--6NYlbfkN0Bvyxp-5kT5PI0anTaEYoEkcOlTMlp7z8iufLqgdrGl7gYuoiHU3tYNGHMONxq_AeZO4OER2IvEobvuBMmLvTMdPHaqt_M3Z8HU1rvkkn6uky3pM1-5Fegz0fHiXXwISWhe_6ig_XHv3FygcCR246BYBcjYBmCWve4vG5L98h7NSm3HMmgCqAUFF6VBxHS0ga0nFD7LqeJHcog2QB0xhhkGZ__yupULMGaKMOI8o7EJQBj6snCj3UbGTwz6yTrQafHOTr-B6-F_sH6B5ZUyWDPDOJaYWnZ7g7CtRBLqqQ2GTRCsg9I00wF2yFw6LJGMqHzTj4OTc9j-YY_M03hS9hf3BKTUzBDDIjCBhF75s-Ldaxx5d54F5ryYVTTlf50HSNRWlFAJvM_2fxXz7Jghb011aEoetsJ2cO3lF6TVlDPHJ_vnvNj0136NesRTKbmKRP82YWIzaj-oqJQFzN1j9Xtt0-G9iGOj-uPKslONpN-gsXF8dC43voqg_3ia9ow0rAr1ifQEEbVqLccubwyCrruN5YJ4PwUAG5gkPE9WOe8U-w%3D%3D</x:t>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=105&amp;ao=1110586&amp;s=58&amp;guid=0000017d035136a985cc529157229a1b&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_ed728193&amp;cb=1636438194550&amp;jobListingId=1007372201346&amp;cpc=AED165184C5D3F86&amp;jrtk=3-0-1fk1l2dsdu46k801-1fk1l2dssu1au800-dc314448be7afab2--6NYlbfkN0Bvyxp-5kT5PI0anTaEYoEkcOlTMlp7z8iufLqgdrGl7gYuoiHU3tYNGHMONxq_AeZO4OER2IvEobvuBMmLvTMdPHaqt_M3Z8HU1rvkkn6uky3pM1-5Fegz0fHiXXwISWhe_6ig_XHv3FygcCR246BYBcjYBmCWve4vG5L98h7NSg9Z8AXV2fljZm2HH2b6JsEJUg6wEwBOEkKD8LocGPxXBXj99yYjeUjpO5HSk42fhnFqiMfJW5YTD3pxe_Jg48gUe4puvnBUw00ieKLPEglnZDUA35ymRV16Z_6tl3WXiZLETOJsjEvRZiQcGqixPh5RZXreNDjnG3gIbPitmX98P5vs_6h5KcBT41fBX6PtvBEGLjzoBnPRfH3WlqVJrkDY_VLnZGafcPkO0VEf9I54bOB4V6pwhvV0Lso_AgrseQOh1YU_URopnqQTqf2nfA9YK93NenHm47nbIZPslH79_-U3qjE-dAowJSFiHvcKx2XvaV6FVNHIRqhuy25NvIXIL6D_PPcxEmdYW1I8Cz7jJuW-d2ZT4J6NL9c5KmEUNQ%3D%3D</x:t>
   </x:si>
   <x:si>
     <x:t>Charles Schwab</x:t>
   </x:si>
   <x:si>
-    <x:t>Software Implementation Engineer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/partner/jobListing.htm?pos=104&amp;ao=1110586&amp;s=58&amp;guid=0000017d02900fa288e32d398d958234&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_2d818dad&amp;cb=1636425536143&amp;jobListingId=1007418612936&amp;cpc=B570179B49F70162&amp;jrtk=3-0-1fk19044au230801-1fk190451hior800-c176c2344bee17da--6NYlbfkN0BQmnM7HETVDFPm94mhyhsRO7u4BdocBYLuhSVOj6qaHkZFU8RulUSOH_KkZ8ynymp3hAIMSGyxLeJ_jYJ4YIN7X0MXZtHG7qwmMytuKaYNWudkDCpqMo6VUOKSrhQgSLRqg_6uHkC0U6qDlPTkhSEXWGeb4rgDiZ-5adsvZmcIVYxE_SIX4lInsk3SH1CVTnDtzmlEdgqNEqI63ibNFJawiWl1zphFHAm46JUNIqGmbrxnYvJNttVoVZUswOUCHiwvlbfA9DuTHxa-1CbW54GyfBXNHLh25KY2CSChlBRzgFx8ToTcNXL3qDvON21OBjNx9QmfTI6BWJB2rYCibV_sX0Id-RtKgc7YOgbay11LRt4b612AiOroTDB2y251uwa-Sn2m7YpUGB9D9toNcY7bq32hgG9dKpWqQ5LN5SQm1nabar1KH3AUqSSYcvNWYSxLc6ecfv8ATEAFwnR3a-wfBMOQPsN7zk2txVRKXM8yUSIQCOUtK89his-258beycQ%3D</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TurnKey Lender INC</x:t>
+    <x:t>Senior Software Engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=106&amp;ao=1110586&amp;s=58&amp;guid=0000017d035136a985cc529157229a1b&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_33f10840&amp;cb=1636438194553&amp;jobListingId=1007005710927&amp;cpc=8D2B7435C06A1689&amp;jrtk=3-0-1fk1l2dsdu46k801-1fk1l2dssu1au800-4b0ba72bd5eda6b2--6NYlbfkN0ANu19da-khu0iE32scipL9wT-xpBwyDcuU4ZPgRtzex03MFjMfkX--eeFms6NZVrs2rHNcJYzoC09f83WgQfaqKZJVl2aEJhVHggNpzkn_xlqMzH7Q_fMiPin6j6MFNu6N7qq4NikS_AWIPtdVY9pnJwi2GRJshGCC_Ac86c5hxvFX1aw7F3svhklSBAjzOUsR2QMOPN75sP89lI8Uov-OkIO-G9_dDCQGK35sJw5sLhBh-09scDoFGvYmOvcfMPyt5CiBuPwgFb6LAt6X56KKb-zNnZUUNbB_0P8b7UvZYHYxl5vnPobtE8ab5qEatoRoC3CTmC0jE2eddUDEl7YPSs89lR19TlE5R1dc3sZXBrwS_8w8a7xrx0quycidlpQh8QCe7agXWjv9t7MjZcyaK3eHtvRlh9Z16WR2gEicETcettbgAs3TTRyoeG25j8vNlWb0CV0Yualys6Q9PRSIyx4ZxGa2mNOWSWbKSxQHgd3uBBPkZLelqq8MjIHTWMA%3D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Skyways</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Manor, TX</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Engineering Lead (Industrial IoT)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=107&amp;ao=1110586&amp;s=58&amp;guid=0000017d035136a985cc529157229a1b&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_aae554ef&amp;cb=1636438194553&amp;jobListingId=1007420222584&amp;cpc=6FDD437F7834ACD3&amp;jrtk=3-0-1fk1l2dsdu46k801-1fk1l2dssu1au800-0693945a03b7b83f--6NYlbfkN0BQZmpL80JLCwCdcvt_aNRBiSGH66qw9sbmu-4MW8dYCAa7F8ejXQOcD4KiFARq31r5AskyX25i-W0hSKaKZvlU7mL6vf1EVW4Er8n5ZOB7G3a_AdEonBFkwiDAeVg3mrJej9KpKGYA_zbaUzea7BfMGKLrRXfFnbX6HblCw5Hq8pZgFVnmfcxarRzLpDIfq6ay3OJYvW0RIX9ZyA_ru0JI-58g8QkY8gtVrV6dCNAIl4GIXH8etMTtO-uaQdyDs9n7V0MK4eEMj53Xo4qrJaAA5plRPF2cTHLyQr7RzE0y4tc1-5waXd9TtSRd5-5VyxehHiT_wJejl-0aaTao0ndCMZ1jUIaRxm3Xzud5yMZOSC3zB5CAE59hMcpUrggz9aUBknctj36fzAC_MC5S_SnLrVt5ZXi7sLOBE5m1c8GVRKzIxX8yEPxMeUvzgCfDHxqO_H-5epv4RVUpQnCSyN7kek9BT9EX0JQj7YCrx6chqwgT1SvuzTAX</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ZimZee Recruiting</x:t>
   </x:si>
   <x:si>
     <x:t>Sr Manager, Software Engineering</x:t>
   </x:si>
   <x:si>
-    <x:t>/partner/jobListing.htm?pos=105&amp;ao=1110586&amp;s=58&amp;guid=0000017d02900fa288e32d398d958234&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_b8eeeb17&amp;cb=1636425536140&amp;jobListingId=1007354458428&amp;cpc=55FC80EBF760BBE8&amp;jrtk=3-0-1fk19044au230801-1fk190451hior800-7bc912fa127fe2bf--6NYlbfkN0Bvyxp-5kT5PI0anTaEYoEkcOlTMlp7z8iufLqgdrGl7itwnSg21KHIOtuVoj_q9GhqyMFGBT2_Z_dsgjYLVBUVlmQeQvDPVZz0Mrohfw62mOoT58RI5ByIjEnvxxJwefZZ3XTZi3Z1ZprfW-hsScmFEANphZuxCmo5tvwIKWVvwQ6JnCuzXoHh33p2XT5D6euPwNEjCIWwPAT-hlrX7sA0nbnLmKdWS7vTL5BSruGy6F6PUvRMCGDBMZbxEqaf07DKYa-7fN6Vceau4kWTglawqTZYIvZYXv3PD09-T8toTooJ6qia03A2VFNrRbcLWmGPCCezNBHikCvyY1SftlJakboG9JH86lUw4Nefyz_HFHAp_yamTBb_TtXMq3l6ycTjdzQMAsEYKr_fhD3820eYpiREDzs4FAeSggPjsQoeVXKpjZtEi84P1nifbah0AqJj_mEPcbkRugw2OnV2urdjNPhMERlfCwkFN0H896Rjt9FesKxOv0Ra7ppB_Vvs54YfRPxIiyqFiTP26YJq031hulRV96rKiAOUWv3QEbHrkA%3D%3D</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Manager Software Engineering</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/partner/jobListing.htm?pos=106&amp;ao=1110586&amp;s=58&amp;guid=0000017d02900fa288e32d398d958234&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_1a6cd6ea&amp;cb=1636425536141&amp;jobListingId=1007420092683&amp;cpc=FAD720BB8CCCB15B&amp;jrtk=3-0-1fk19044au230801-1fk190451hior800-c7ca0756db1b838b--6NYlbfkN0CNTaigg53tgKMQQsjdGlhApYl6RSsbpQl6QWYzGuod7wABAFGU2Gsp51ZfrOerCIlBvuBpBsrfm6XT53Wdxz49-q37HQDkplldIzyQpVZe2ixOzikjbSgXx8EOggTpSKZYod08Fi5MR4X1LG_oVaMSLEOQpdNcu8m_5Y7tyI9JpwnbcQp6EIJa4lBE24Uq-yBku_USeUDt6JSyaq7dTrOTPnfAujaMdrIikkvVrzLP6mNmrndyqJHGDwOG0DvvpT1omaBG6Ii9ZO2nMUDLZ3TpwaotdHS4DZN0bDWsR48PeN19oXIBIYBafPgMf5izpj9K09JZcTxT4R-z67IvlpFDKb8aI7c_dK-AJo1u_a3o44IaYtLCEX2gZdYUSkiM-WBNdCcwIMtHdzB8FOu4f4u-LqtIScYCXGPWU4Tvk2J02XT9d9eFsjh19-HDGoEjzx4XdOZLDu8N1zlpbfYW-12rz_rBQ0l92fR9QbwqGjo300spNkT9mWvSGVeltZHUjkOZr12gQ7uv3Zg4j5iXboREe3qrGCzwx7ylqvkZm3G22pqmTIcYVbWqGjr7p8XTa2u6GisTQ7Mt24qrTeOrCuanogxGID7IsdDFAsXNHXM_z4VyquCHSDiZWpqduRNoXurhNrhIWIHBLnAcN7HhnO7oQBNueuFDAPc_lPouAwNkmlxL-k0B4LwsR8GgtWUNUtQTWbtHqbUVmb6Ibvz-H-uWUgKWtic9L2DIhA6uwwuS_ZFukySoIFniW8LT_sPm3HbQ7lzAm--ptVA8Wd2rsKgM061J0u2HOJlrg8zRV_d4v-Mu8V0vwFXKI3HSjnxNVFYNTinSeTPZO0HHUtB0D4MlXLO8XEVWiDj9k4mhVtRl-rEvQDx0TDRtxH6lNdz1utAdgF94RwFuSjqNequQcVBlyBT3by3PtSxyAyqG2sb-fV3pl0l8Zzj0Ntlc5uGPACNqXEQJBSYJfRsX0RD9WbzDJBem5SC4SjaxymYLzd95Nw1BhEnEZT__We9bTWMZWrd04RkFgn3BQW24bW-WkC1kHZcIHWztzN1JYKGyGF3m9gj_6um2BrQU</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Cox Automotive</x:t>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=108&amp;ao=1110586&amp;s=58&amp;guid=0000017d035136a985cc529157229a1b&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_aa561c80&amp;cb=1636438194552&amp;jobListingId=1007354458428&amp;cpc=D7FE8E303655E3F3&amp;jrtk=3-0-1fk1l2dsdu46k801-1fk1l2dssu1au800-7bc912fa127fe2bf--6NYlbfkN0Bvyxp-5kT5PI0anTaEYoEkcOlTMlp7z8iufLqgdrGl7itwnSg21KHIOtuVoj_q9GhqyMFGBT2_Z_dsgjYLVBUVlmQeQvDPVZz0Mrohfw62mOoT58RI5ByIjEnvxxJwefZZ3XTZi3Z1ZprfW-hsScmFEANphZuxCmo5tvwIKWVvwWJU3QMUUOQ-jHbaX2K2BlFzVoFYfOgjFWWwEXdK5iXWvvrGldemhto8_PC0aBcVnvUr46nEH4PusKavZC1rk_UH-G0RgpFQYnLIHrTns1A89OBPBnyjxvSiiwH8kPpD9zdrs7F4HxijOfE0yZMH06zRBOhsLcPzSZTeIEiYuoMpE1Ml_V5mw2jKNlDZ_LS05G03oluvaF3igZzzjAEULEqEiT9uXUva2YF-Bdnm11GKGrI-OSGQHUtUYAt_zC6FtktD8RZXRrCMFwGySopA2vrAgx5DE8XzDjm7_eFWlX09SufeSyMwFl_EXajuIGMqCAGtd2Aq5ENl_BFO1RInrzb5_0NnqcX6i_BhQ1b_fVW-j3Og9mws5rg8Op6kkyUjvA%3D%3D</x:t>
   </x:si>
   <x:si>
     <x:t>Manager, Software Engineering</x:t>
   </x:si>
   <x:si>
-    <x:t>/partner/jobListing.htm?pos=107&amp;ao=1110586&amp;s=58&amp;guid=0000017d02900fa288e32d398d958234&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_0a71702c&amp;cb=1636425536144&amp;jobListingId=1007352307668&amp;cpc=608BEFD8E68346F1&amp;jrtk=3-0-1fk19044au230801-1fk190451hior800-0aae5396c7d9c5e9--6NYlbfkN0CiRNM7CVr8YueLFKlzwbFWI0o7IjV438l4sVrvKZ0flkywQJjHRBleObb6D711MblzcbPJILA7DbaiMpvVPVNXVKdscBuUdls43BQlbviByGaQvJxmdCJmiGoEoSETFAcXKD9y7FSGw1N6ByKMldrbEnkm997vRtC9gHayGMdYKHfJjXX_2puSQAkwQwpTJJTTqqz4rKsE_ReSs-Vs_VmT7l9NZCuSowxXX1Sv_lLqcGJLztrx3f051zqp3wCQ0QkFPGHqIWFiJqi-CVhWx_0aL8TPQJ8JtFZ78JSxFwCxvu1VoiQdK_M2sl8ITMII_yWTzA1vm5z4_hReJAYAl4zaPN95z9Bl3zFI08WKogXm9W-ymVXiEzHINwl0NFFvH8E4_jgQ7-pzhtr5CqoBS2J35OjMJhVzGG9d2_0ZCwGMYKXyz2o6uXgwEv4lpOm4NrGQmsp_AGSpqBcQ7SbFm_j6kanrY6dvkI1A2vrCVmNxWJBfe01u-ea_y_oEaoZdErn66hGs_VQvrQ%3D%3D</x:t>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=109&amp;ao=1110586&amp;s=58&amp;guid=0000017d035136a985cc529157229a1b&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_8db74c84&amp;cb=1636438194555&amp;jobListingId=1007352307668&amp;cpc=70E6D4E49C80165A&amp;jrtk=3-0-1fk1l2dsdu46k801-1fk1l2dssu1au800-0aae5396c7d9c5e9--6NYlbfkN0CiRNM7CVr8YueLFKlzwbFWI0o7IjV438l4sVrvKZ0flkywQJjHRBleObb6D711MblzcbPJILA7DbaiMpvVPVNXVKdscBuUdls43BQlbviByGaQvJxmdCJmiGoEoSETFAcXKD9y7FSGw1N6ByKMldrbEnkm997vRtC9gHayGMdYKHfJjXX_2puSQAkwQwpTJJQ0nKyhKTR49WAs9XU5uw75PKWEKYUQhzuWe44lvJNx7-7GzVslpcQUcsy7E_SGzXGSG2aOiOYqkh84CehAE3XyEvAzzeE3Cpk1VoArvrRy2tdhMFPYKxS-fT8HRS8_wJXTWsjpRTP4M69QX1o0zFUQPXLSwE6vdULRi1W468cIom0-fvLAQG8sis25b_SCFyYhoNaba0mSIWhiD8zwFsge_Mj5RG3RhUUCrPV4l33KUeTfp9dzD1CBQGOhgvhrLxWdWKmN9bU5NGJYGBfN2fjEgPb95PqanVUhU6k4PC8nFG128uGURLrxpz2j7oEA3drdGBlEeaphAA%3D%3D</x:t>
   </x:si>
   <x:si>
     <x:t>Indeed</x:t>
   </x:si>
   <x:si>
-    <x:t>VP, Software Engineering</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/partner/jobListing.htm?pos=108&amp;ao=1110586&amp;s=58&amp;guid=0000017d02900fa288e32d398d958234&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_01468c71&amp;cb=1636425536145&amp;jobListingId=1007323856599&amp;cpc=25F7D4ABB6558D0F&amp;jrtk=3-0-1fk19044au230801-1fk190451hior800-8320d025d4b8b065--6NYlbfkN0CiRNM7CVr8YueLFKlzwbFWI0o7IjV438l4sVrvKZ0flkywQJjHRBle1nJQGsulJR7-eOrTKHA5nQpCqy8U5_wEAKoeKczoK7stroi7WDMiaNI4eXWjsxR6ugl2744_gl2agzJ50yZqIcn93_rlnHH4LooKi0bM0tstoujRzxqDF8qJvUPOwmvHlhBaCSH1_nX22yKgjLo9N7b5XJMWU6aRhWzzEmzmQsw0ZY_GgDvi2LicOtLmoVJ_nruMRSgTVjHd82FAXHy1UeB-sa11niDb7WFq70lgp8xyunbgPqAjocrKAzfnNte0H1IDqcQIfhB6twW_i76CiNoEBeVsRPzKvfUZiH-Q0oXte77FoyG2CRuLEK77lWhVtLe9N0S3u1xuvSD4pyg9KdH4G7Ut6kn4WWXMU1LNCoLZ2P_vjZMTGOFYu1Rmg7dHBARpW8u3kYehpmkTCEdXIXBvXQYWBCDyMhg0PTnCTeoQng7UWgnD3YKn3z3kkqfzy1hsjFCn4ZUOnB3nqN4p3g%3D%3D</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Software Engineering Manager - Candidate Management</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/partner/jobListing.htm?pos=109&amp;ao=1110586&amp;s=58&amp;guid=0000017d02900fa288e32d398d958234&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_0bffca89&amp;cb=1636425536146&amp;jobListingId=1007393606066&amp;cpc=8507CEB59E1C6AFB&amp;jrtk=3-0-1fk19044au230801-1fk190451hior800-6a1281cfb892ac73--6NYlbfkN0CiRNM7CVr8YueLFKlzwbFWI0o7IjV438l4sVrvKZ0flkywQJjHRBleObb6D711MblkYOrrd0wd9v5_7o_xQt2YKDiCMLE8hqmtbgvXx1ctJtEYa3VT3QoLJb10pVljm6gioiYYe6B8OQqprnmmOHcN2tVxUv7GoZx32qK7zX0jn5XJmt0xNaQcx1K0Z72gGhAyarzsRDOrK4Auu3aTZADdXRm4pqJR3ep1OmIgEKnv1PitRRrsGAMcXXNh9sACJoSGHujvtK1SzPkRhw23L0bLAtC9GwhpyX_6QttK47yrdk-0busqzdx7Eh0ZBH3r0gAyTpFWPjnvaeV9PcThcktf4Ch-ax3IJuqRqT6q4HuYDR2ISgSb_wiqaSGbRubemNQAIyEKc3vAkR2O8ySqYhsu2OXkkGdUzwoRSlisKdRJWAOEYkCrPo66njLo6kNXGYt3eJBUPPTurBoQr1gwqPK8TsaziOj1LSKkov0u7ct_f9o0spP28bKeHN5osELVqXewfgyHvsIzKw%3D%3D</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Dir., Software Engineering-Compliance</x:t>
-  </x:si>
-  <x:si>
-    <x:t>/partner/jobListing.htm?pos=110&amp;ao=1110586&amp;s=58&amp;guid=0000017d02900fa288e32d398d958234&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_07815e05&amp;cb=1636425536145&amp;jobListingId=1007383856560&amp;cpc=22ABB673398E21F3&amp;jrtk=3-0-1fk19044au230801-1fk190451hior800-73cd7c80cf73b565--6NYlbfkN0D-HIqnNg6Mnea-pJAft-hE3z400wxCVxUkTfHd-jtFaC_msaJMG-MJaD8a4EGrvJDCyyNAADlMg7sKn29S_H-qApJDoG_krw3JnclygtRy0C09SgayBras-img6NChrAK30ScF-Qez2OG4xvv2nGSoqTEBAu_g8AZhNn5ul6JbQt0-hQ4WWN-GF0GeP784fe_qwPROgzYxOOAyZ-IqJ3EQIX2MkSOffbid-QNOjMP7r-AG44gnubkvj2FLRabdt2UAS-UxqSeoleJe8idWWBrpzSTM6Gogp5FIL8VL1WlfTY1HexLeHiwaQJcPSelaQbdRKnwPJ3iGCCBHpL1Y0JkzKSsG9s76NvJGF0GH7qNGXBgVbKRTVGxxxlNcqAH1DUU1J0a-GgUShgB36NSQthSr5OB2djPT5DBZuwzpyBuF9UwweHsnMorCqS6hcaz6qzUE9TCLi_5KL5n8RtntIynTAKszYVbPBW9_5PubUE8-BQW2kHh9NlQnPcjawAVpziZGbQPUORjbZg6YYJirRdJmk9rcM2o4VUd9GtzsWxrrCP5ulVm6NGoZt7t7fvL2EtJuhP6SBL7GZBji5vhAYSho</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PayPal</x:t>
+    <x:t>Senior Manager, Software Engineering</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=110&amp;ao=1110586&amp;s=58&amp;guid=0000017d035136a985cc529157229a1b&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_f699abe8&amp;cb=1636438194556&amp;jobListingId=1007380632329&amp;cpc=56632219D727AB75&amp;jrtk=3-0-1fk1l2dsdu46k801-1fk1l2dssu1au800-4d221059ec140963--6NYlbfkN0CiRNM7CVr8YueLFKlzwbFWI0o7IjV438l4sVrvKZ0flkywQJjHRBleObb6D711Mblo1WehR2exmQCVp5hjPYq5KZLOvFjOHQJEl3wTL0ENM5TfJRcmM-dS6Cv6SDRlPEX3wGyEKQsg8IsQRN5ezc_9rc0AIh1fkTQ6tQLcq3SqWK5HH6molRVQJ3ud8ANbyv27xoso7pPB9pHbCz-2bRDBrCTCun9bdAxgNuto7ajxXDLSA_1ldBeWmCuBcSfMZdWrDs-4PWTGX2maIwGsE2PRm6cL2e_FFdL2my6vRwJTS3K9sZi7fA9fSgSsKRn3EdPyBEJ_oQO_U1vs6tN3bpbtIAsrLXk_1dy8oMyJxsyXEZ7wRPxNSYOgeQwlOjHNfAnuDL53MKGRX956UXi5g9Tcs-Shmvikfvx-aJN8k09XLtJEXsFBv-lM18KJzqCor2y49aOUsGgMGh5O7zUF8sanuOHEsgIyHZp6WXFQJLGzFwt9IFqfNR-Vh3BnSNSLQFS6cJWESj1czQ%3D%3D</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -507,58 +516,70 @@
       <x:c r="D4" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
     </x:row>
     <x:row r="5" spans="1:5">
       <x:c r="A5" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
         <x:v>3</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:5">
       <x:c r="A6" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
         <x:v>3</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5">
       <x:c r="A7" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5">
       <x:c r="A8" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
         <x:v>3</x:v>
@@ -566,13 +587,13 @@
     </x:row>
     <x:row r="9" spans="1:5">
       <x:c r="A9" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
         <x:v>3</x:v>
@@ -580,13 +601,13 @@
     </x:row>
     <x:row r="10" spans="1:5">
       <x:c r="A10" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
         <x:v>3</x:v>
@@ -594,13 +615,13 @@
     </x:row>
     <x:row r="11" spans="1:5">
       <x:c r="A11" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
         <x:v>3</x:v>

</xml_diff>

<commit_message>
update with all webs
</commit_message>
<xml_diff>
--- a/Job Hunter/JHClientTarget.xlsx
+++ b/Job Hunter/JHClientTarget.xlsx
@@ -14,105 +14,126 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
-  <x:si>
-    <x:t>Director of Product</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=101&amp;ao=1110586&amp;s=58&amp;guid=0000017d035136a985cc529157229a1b&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_9636ccf1&amp;cb=1636438194548&amp;jobListingId=1007338908659&amp;cpc=50CB34463567876F&amp;jrtk=3-0-1fk1l2dsdu46k801-1fk1l2dssu1au800-e704d3e164c9825e--6NYlbfkN0AOAePQAgQDSX6T10l2CdlahB9XGxXsykaMCL8scOYOLJPWT3z1EvnGXnjest1zb4NIA28Gb2SzRfl33MKrUwrINUzj2nUoXN__JKckXz7bi4x6ePtSMq74h6rPUrBsWou58xq__LzcB67uLL8RoGaFPe3qTM2EqaXhxPCWnObEjoXPpYFwH9Gcvc-SmFUkgqzPZD3Z8bBo4Ery1c2Ev2-lanouhjCXHWzRpk7S80ioueNkYvi-gCR_ZH2_Doi70YVmSCnBBJkcTq7fGCePI9zIGaleBCXPitfK5h4XqNkohGGg2J02xLpFvYspuox0FXZs7okzNdpVecpbezNKP9GvwO6HI5_1jGenI8Wq6BWWPZzC0u1NBBLJaNQZeapDygVqA5Nk0f7c7rv-ONbGi6XrXsyoHx9KvpJ2X78y9FbOy0aPZh1u9_Fi5ArBk766i1n-19WBDFL4RUfoUKHZYeCUyshBSlVrGrXW8qL6vDob_Prfua2_0O8e</x:t>
-  </x:si>
-  <x:si>
-    <x:t>KIZEN Technologies, Inc.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Austin, TX</x:t>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+  <x:si>
+    <x:t>Senior Accountant</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=101&amp;ao=1110586&amp;s=58&amp;guid=0000017d06c3e4d285a10d0346a6b2e4&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F2F6F181172E0D6290C2D13E89699FD&amp;ea=1&amp;cs=1_9489ae42&amp;cb=1636496041676&amp;jobListingId=1007332495127&amp;cpc=FB91BA2009EB6168&amp;jrtk=3-0-1fk3c7p96u49i801-1fk3c7p9ru25n800-813adafdebc0e24e--6NYlbfkN0CFheh7eSUSHEwDr_W6ox7XeCFcxwMCK__nsBuF72--9iLa5ffHcde-fUzwP2p0dU6sHaEN_fyln_BLwf_1lFfYoEQkNRFtBY_4vr_CHOrJvodoK7Z_MUciXE1A5fdQ-MCDAD2WmNGM9dTDO-I67e0BfJtdU0nn0bZLp55N1xcy_qQcknKAP9S0JVuupXhSU5buWs5b-Jd4Ajyq1HilTQ9JaXCmn4iCyBzzz-PW1FaMfU66x11j4VkswavN6d-vc0c8QtKedrjn36gXPysNdjNqXumAy0RTqmkgX0LLX0Rbn0MgqVi8y174GST7s7J34iyTyMf1H4GhHHg7hiSOKuOpKLA2pC7v-k0G7eu4BmVRNya_6tgv6_TxCUK48sPYdzw-wLW3avEkWA5QdSkDCXa-8MBxBEmKw5HYfv8X02KO_86YF54PlHdq21Gp0kUBF8zQmBvUPcgVbIwXu1DAQ67xQXC8pjind4ln1FE2eSREfScsKxYCPjN5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Diversified Real Estate Company</x:t>
+  </x:si>
+  <x:si>
+    <x:t>New York, NY</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve"> Full-time</x:t>
   </x:si>
   <x:si>
-    <x:t>Expert Associate Director, Software</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=102&amp;ao=1110586&amp;s=58&amp;guid=0000017d035136a985cc529157229a1b&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_4ec789be&amp;cb=1636438194546&amp;jobListingId=1007355118481&amp;cpc=097AB8C29B9A33B8&amp;jrtk=3-0-1fk1l2dsdu46k801-1fk1l2dssu1au800-ac7515175a77f4c0--6NYlbfkN0DoP8nG612n6SaIo-6cBFZ4ajKscvbmOmjTSQxsFZrL9I2eucWeLTh49xiULvC3ZXqLP20PfTxmoV8V6Uqx2Mavwfd7Ibmkq8SvUom5lH3D7p_0iIOw6OilIpYctcx8yiNkrrdzw06HVuZrxrUSoBrUIDaDUKJTsCqNASSk4UFUVm4arcO67DMj6s1__FL5KKxairjH8exhEdXqA2_7FtIkCqKcV0ulK6ui9OAh3dU-cwOKqMjrJD0ycfiZIDP31Hrg8WSbX7XmNqfB_Kl6dJnq3a7gGOUTMXqjFM6fKaEwPLjszmiTcSAGtJ2vckXP31_uCdzsPTX3mY9eHIOIgrWftvrQ7jsjxap7cwc5dfuivKWoICPph3OeeybsWltPqZMCfIl6J9zNs4OYuzkWe3BRYuqA0-xkKWllwc9xeJQPohL1Jvu_B8SzAU-C92zvdwc3dAMN6k-1CIXv4GOCGjYdViDsWFM8c9g-RrtVKqs2faukh4PQKDyvWlrAU7-OZCXcCeKBwURkiDAAJjnlU8EGtHBg1HnPnNwiyJDIKmp5Et7iilGqEYraJeaCZ9_ZEcpRaKwDcVWOL7WrFobG5L5DK0fND7dca_AiP0TAf1xacrp8qp3es2eYhQGfuQy4G2dMe9U1Xvz6J7fP7Iz5lm14WBxJzw29Iz0BX1CXYpIybTscqlTuySrMHzxcOKJQ-Ezj_leBB7FmRw0fpaRZkaSn6v44LpsnNgq1j0TegBfZvQnuKqDXQTkMOS0XMxU8-y6xhXRNFEQqqbBEzmj9PI6cFaaHKyEQA4dvmdqEgaLTNJ8rrHRrYcWZZ6MSq6F3qtw9aU7Yr8MlRpYtIScDWux46C2HyiTHlICP_YiAlVCLrssWeI_j1YbFM9rTlvyxmD9RqyW9eVSderyJ3VOrw5TOvNAdKVsK78U7n1JOaGs8EeF4jc_tU8W4SR5aQWw6FuhoMkgRC5jH2kYa_NkmFT3KhEF-UQ9HWxXecxuP_lBr8DyYl8B8cIVmAJOCTXt5tPBmFM1T6BOE-XHt15hQwJ03</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Boston Consulting Group</x:t>
+    <x:t>We are seeking a bright individual who can assist Controllers on various accounting and investment p...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Staff Accountant/Senior Accountant</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=102&amp;ao=1110586&amp;s=58&amp;guid=0000017d06c3e4d285a10d0346a6b2e4&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F2F6F181172E0D6290C2D13E89699FD&amp;ea=1&amp;cs=1_a79df394&amp;cb=1636496041676&amp;jobListingId=1007165460313&amp;cpc=AE9297225A38C224&amp;jrtk=3-0-1fk3c7p96u49i801-1fk3c7p9ru25n800-fd094cdc4ea10606--6NYlbfkN0CsiqsuAtvdWzPb4b_7B96DIrhySPzdv4FG7XsbZH1FPtDztzrDmbS4BNMha0xZ_qn6gPXZSI82rSnA3pJ7n0waD8uH5tw7SFJVfGR3lWzhwEJhMMLgKQlybaA2_q7THK278rx0GDQSsTRpatwfz7uKSfZ7sK7JbA3p_3DchLsugDILeCDgwpi_StoW4gyq8WbyEvrs3x-vb5oRe49QNkyHnBMWU21GlkgzSyLx3HLSMmWUZWvayYkl_FGQPaLI2sMLZ7FJZ_Q-O0ReltNMzIN4T8nU2_5yJYel4CWaEc9m3xunMP6ud98EkFdpB2atuaQvXNJgea4AKQNi7RBY6CVxNQ3bVZ7jmPn3X0_NfA-fSxvlsH7GGRKM3G2of53rmRsgqzUmDfqZJ-KOymHAjDlRA3xx1Gf1yCkjdb61OGladmJh5jdPYguXST2NHFbhoc85pJJAaSqtItpDi0EZk0t1tT9r6EHfNrYhoW-LSscLp4-HvsGm8G7vGao9RJGY45vZvNKlwY5ghA%3D%3D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hoberman &amp; Lesser LLP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hoberman &amp; Lesser is a mid-size Certified Public Accounting and Advisory firm, located in New York C...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Semi-Senior Accountant (Experience Required)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=103&amp;ao=1110586&amp;s=58&amp;guid=0000017d06c3e4d285a10d0346a6b2e4&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F2F6F181172E0D6290C2D13E89699FD&amp;ea=1&amp;cs=1_2da59344&amp;cb=1636496041677&amp;jobListingId=1007377411152&amp;cpc=A50357DDA226FF0F&amp;jrtk=3-0-1fk3c7p96u49i801-1fk3c7p9ru25n800-a94848b4b7fee52a--6NYlbfkN0CtwOkgDuej6vPfWODMxjOIyNEohQmdYMppGq8y8dOpBqaQGVU4tVOVpluzlhQ8N9LO-I6z2xgv1D197IRt-TjPdzURxQSNYf4zbzEx4vIeIBcdol_xYzrCecFx5sL2vIV81WENKyi9tqrsmGoj99V347IKmefJvbTUkrg7NhamIsO-oF1wS04SJ03UyZMVQbO6AOa7pg_t5pXaI5-gHywrEokmrkKIbmLOoN9oEYJDWOM5hDdnVANqWEgRqPvbTTa02efbk_WOIUiz64T34mhYA_JADJ56Q8ME7NYKQeM2xhaC-AmE5HCLkd5dgMrn-fWOeEkBdRAL-KRzFZ4-7gWmnHg2lzKPRzTUwbpuw0nVxtwhcfWaeLlEETfqBjVsZ5ckx8tzAEnVo_QdUydJm_W-LOblpwS8nx-jXO7pzN2wJC1yxE76Xgip_Bubx7i4IPiN0iWSAVh_J9fFAEZA_OIVQ_YFM2vUId6HYaqo8lSPRR9HxvPkaFuYdar9ZjfAz_SPl3woQ8GewvMyeRKU0A-0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Raines &amp; Fischer LLP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Our firm seeks an experienced Semi-Senior Accountant with a drive to interact with clients and learn...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=104&amp;ao=1110586&amp;s=58&amp;guid=0000017d06c3e4d285a10d0346a6b2e4&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F2F6F181172E0D6290C2D13E89699FD&amp;ea=1&amp;cs=1_a2876139&amp;cb=1636496041678&amp;jobListingId=1006936933899&amp;cpc=241359978B7FCDEB&amp;jrtk=3-0-1fk3c7p96u49i801-1fk3c7p9ru25n800-6399f9587839b797--6NYlbfkN0DXIqEcRagNjM2D6V3zaAir9KeCGU1qEKArEmDBSQxJZKbydGVUJc8eWrhfTOu0fQHkso6us9haOYM65fEiSkTBrQAAebCYVJQqrT5-TfXHugi_6PP0CP9Yk2F7EE8uiTNKEwew6tAjpFWrtSXbd3UjMWcTspdova90dfwm9EGByKs4R1Vz_kQYU-hXBJFDHBI3y6XVWlMT-FzPHhcvH5L6lcamy0YG4g2JeEfSed4L4EwBDh9iuhdL3gV_XtAJTJgPQEW4nEWQldAMJkTThENXCFREBNJMmMGLEGI5f5VjUz50WZElB49D0d3M_zGI1X9OJGJTZfNwk7EJFMeH3ka09EP5IlPiXQs7bFKZMTufSU6oXWl4m_8RqHURu9sXPY8JOQGlUNWTSVSUbQupVIqr04GhcWB6Ixk75aakmocRiKQchq-bYzLXhcoUb0xuuLkDflFDtgbzIhvJAUExB_qWndPGBF-ekLeNEEYVJQIE59LPfdbrK4Pm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>New York Design Architects, LLP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IMMEDIATEProminent 25 year old Tribeca Architectural firm seeks experienced Senior Accountant to con...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=105&amp;ao=1110586&amp;s=58&amp;guid=0000017d06c3e4d285a10d0346a6b2e4&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F2F6F181172E0D6290C2D13E89699FD&amp;ea=1&amp;cs=1_d999abf0&amp;cb=1636496041679&amp;jobListingId=1007401869275&amp;cpc=F4CC4721A073827F&amp;jrtk=3-0-1fk3c7p96u49i801-1fk3c7p9ru25n800-b7442ae82af528f7--6NYlbfkN0DAwgduWqBP7ymGN-lTADpinz2i-23XbRAyg5ywqS-MDYi_s7Thtk4lX7i5GAqNpXenlvJENKGQs6YdvXdI0JXj3C9Pv9Jf9N9UZaon4gyRN445XQP_OBYAuEnCAaaY8JdGqvY_ojI81lyMfn3YwUUaQbVXU4kfX1S4sqrSmIE-1umlzCB1LHoJ8rl7-LqIrSgtlrg45IafqtNOvJ4w2MVzF4I-k6CkNFOUPt2X8RIq2O3KBF03G8I0YMZqS2mT9p5nwRfIMR3g6G3YluDNa29i5I_qG8BCH_6a5teqzu6zsxBACLsFxXZ2C5ovRA_S07OR6EPASoNU5omzs9zn2Z5ZCAmQ7Cf0jsGjNpfp8E48uUvwqWR1YUX5sGSVZ_Crs3U3NliT0Xi0AoTU_p2soq5jLnh4yh-L3A6d9_hMwAyJ0_JvzDjz3qHkAWMRUPky7blkSLF220RD7Xn2e7uj9h9IcvMW5yWfmxis7HWYT12yyHiG5EQ3cgOW</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Toscano Clements Taylor</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Staff Accountant Associate</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=106&amp;ao=1110586&amp;s=58&amp;guid=0000017d06c3e4d285a10d0346a6b2e4&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F2F6F181172E0D6290C2D13E89699FD&amp;ea=1&amp;cs=1_7f6161f2&amp;cb=1636496041679&amp;jobListingId=1007246985322&amp;cpc=B3B142CD6B71FD88&amp;jrtk=3-0-1fk3c7p96u49i801-1fk3c7p9ru25n800-0df76712f5386efc--6NYlbfkN0Dl8IMvTlUpyY0fNxFFsmnRGIkWh_m6VxgQLP5Pfft0j792K-wCd8TjtNXFufRtbOXvp8L4Iivi4t6jeY4rqErxOuu_sNqmEJ043nHL8YepJZY5aK5jtVL885a5FKNqO8tjXOkb8AavjXank3WKoAS4kmzRrFflP80oAd3dbU1cE0xoAW4A2SxteEd8CiijqSxOhP2ogmUnATV3iI9v1JZFFzSevUehTyUT6zijg8xksBefS3FYV8EPEz61PG8SxO7ywlJdeOQKal4S6C0lmIRRP0Pjza8WZamLVScl8wHyxfKP-dCkIZPpuuT0ouYh_OWCioUiFDW0s_gqcqAovlLSI6NW8aUa0Nx2V8RhpmuQwQtY2RN8XyIpIeBMW3pYcz5_0L0yhoNv1wnbGbXbTWqTcGznmSCWthXKlTfvPx_UpNg58CJcyb1fcTw7Vy16K84VStewxmMY7-Nlt6l9osptwZikHAcq8H5D4wcmGcDaTfDWAFn4UUaUys5xdFXKFLMzZtrZzo-DZaI5svvO-ec-CG2a3d9wPGVuMc69mn6SVWDiM8Z6OTcy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OTC Markets Group Inc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OTC Markets Group Inc., operator of premier US financial marketplaces, is seeking a Staff Accountant...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Staff Accountant - NY, NY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=107&amp;ao=1110586&amp;s=58&amp;guid=0000017d06c3e4d285a10d0346a6b2e4&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F2F6F181172E0D6290C2D13E89699FD&amp;cs=1_61620436&amp;cb=1636496041678&amp;jobListingId=1007399629954&amp;cpc=F5D43257E3E73E36&amp;jrtk=3-0-1fk3c7p96u49i801-1fk3c7p9ru25n800-861dbb5ff383c8e7--6NYlbfkN0DN0uKknIRIeHRZyobcf3FRiQlpXuSIu20Fm8rTPpuaEScs5ILohoWoCsyWJ4d6sf_KW_vToU7N4fR9jkXdWAhk2qns99GxRgAm4Ncz03_i_D5D648u7H6didrRuJFofLtP1wfWe1p7cQ8WbTdBVP8i9vyKgc7LHeoWhcb5f5OjABXhO-PoBwd04YHk2YeyJBH5sP-ZBypBqk69yxADBexPUvUOZFn32V5hddiYXUTqucmL3JHu8HOUEeQ3BuNDIwIsdWSxSI-h2RMwnDPVkjgJDa2IDzmCxVF-nE0PtJkjuT6Ec-jv6e_aen4rRaKKscLyreBFpXZIt5frj5Si1wwkHe2VCK3E6rzI7kLC4hKAIZoXODU8uY5O4AxhZ40KyldPHtjCxS1sdYr58OmN3kZT-bOroPG7ZS4Ow5VSF0gvvxOpolPOgiFP-7laD5eO8cCplUf9ssOitnryPir2uXTvRsdwtPtmeXKnpT0TtzqsiWOcs9msbGpiH63im6GTr33Uufb4bSbFF-DQGu9sVTSCqyDzXACGrX3_wz7r-DOg5C_o6929tWHRnZRbT3WrlC5rolyz6EzApPYI__JhZKJEBZQpb3rwX4zZc8c_3bVlZ5VFxIjdgqcYdHH6HBPTH__ZEDIDLv9XTNLNG2aQr3pnPg3Gy8peE-MLstZ8lcTJlSYp7W-tMYQB17GAcoSTJABYo7wRkXt1SqVDMpMkOZ3LHDtfRYyFZW7oYEhtNekfHST4csWnWfQ505Xa4noKDvhHgPHbzSgvKCyFiL0JGRMp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Your Part-Time Controller, LLC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Overview:
+Either a Full-Time or Part-Time Opportunity
+Your Part-Time Controller works with nonprofi...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Staff Accountant</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=108&amp;ao=1110586&amp;s=58&amp;guid=0000017d06c3e4d285a10d0346a6b2e4&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F2F6F181172E0D6290C2D13E89699FD&amp;ea=1&amp;cs=1_3408bc06&amp;cb=1636496041681&amp;jobListingId=1007363832948&amp;cpc=B6E9EE473EF69035&amp;jrtk=3-0-1fk3c7p96u49i801-1fk3c7p9ru25n800-886b0e4851fc04e8--6NYlbfkN0Cy6Y0fLVKZlaLIH3HmWBB-umnKJBe35kIsW8Zj8Ud66Iy5GzJSobzI_R7kfD5BXSKa2ebF0B1PRkB4zvGh4nTs1yvmebXlDifZ2zfZmYk1SsmHla3OxBDOtTljSod5rDO4aH8LccOirqFBiJo8teYdkOshsBtVFE1GHhpocFVgLExkLbCoZrYp9LqZ-T8Nd6LlYtdls0rueEndPTa1LL39pjYIP1G4naNC8vh31ZKEKjE06WfqeDX_Zyhsv3NBbhAQMlpPRz3yYJHpLu5vsvb2_SLnJEegSKYgbcdEQ1DUyCdiFvVFdBrbqgvRhhnN2I8Xv3gGsFeWAQOhpdGjYxTIym-D4-5T7JQKYPKs8Htnx6_ku-VTZnfgdxcFUWpaCFSwPGX4OBKQ_O26Pk44zqbBwGEV0A2rMh3qwdg-bwSM4u6wWxISk2CPIvH2eT2jXuIRaV05iw7yvXERl5PMCkwExaOs4C4mZ82cSl8NuPHhS3xKQBPbo2NMX-GyYvqWRjM%3D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Biz2Credit Inc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>About Us:
+Biz2Credit, a Series B ($52M) financial technology company founded in 2007, provides fundi...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Senior Financial Accountants/Analysts</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=109&amp;ao=1110586&amp;s=58&amp;guid=0000017d06c3e4d285a10d0346a6b2e4&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F2F6F181172E0D6290C2D13E89699FD&amp;ea=1&amp;cs=1_ed62c637&amp;cb=1636496041682&amp;jobListingId=1007403100390&amp;cpc=90C4CD7F4113B630&amp;jrtk=3-0-1fk3c7p96u49i801-1fk3c7p9ru25n800-c0033c647f66c986--6NYlbfkN0BdX3W3WyFVN-ulM4iCZnMv8qZviPHHsAQc8kaRA1cR_dlcOeKDcEnDnW3QqNbPVkcEHwI252y3V0nuy5NmxzzBI7hIQK1KXoWURrcZsr1i-elYoBpIfjRgGahKtZSqqsTsrKG13muNqcOC9M7MNrzkJwUD5TkcDmJtn592F1Qdy9H8nftajfE8JRpWeXZ5OppH2ESCxNNV-BoHelovaz7IMccVqv6nrKnQBdDq0w-14zUTq5pm5FaiKKIPap-BXxx1p8Dek9Z3o4j662kmULJvxgfrPVzVnaN-yPo_7hW7KXM9rAfHei5n9AI620UlEi2reCNgFUcs6e40B962VTtZNroIU8CnLILpAZVwkmeQn82avowGk9HP4F7HsLpepPgO7B5m1vhenjKs_YJB7xIWlL_bOPFVv08oouACdDQr8a_9IaB9DdkHPIWQ5sbFpfFvbFiusgIIh68FnjrinshOhM7JNETxf61A2DGaOfL-Z_nInn2plEI6PlcrnV2cdljKfMVn9sBE5NqYhTXVuLe-</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Access Staffing LLC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Senior Financial Accountants/Analysts$130k + Bonus(Hybrid Position)Two of our largest global and exp...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=110&amp;ao=1110586&amp;s=58&amp;guid=0000017d06c3e4d285a10d0346a6b2e4&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F2F6F181172E0D6290C2D13E89699FD&amp;ea=1&amp;cs=1_51acfa2a&amp;cb=1636496041685&amp;jobListingId=1007407883193&amp;cpc=0AE43CF55DD5119E&amp;jrtk=3-0-1fk3c7p96u49i801-1fk3c7p9ru25n800-b58bd8b0623b94aa--6NYlbfkN0AVmeVdBxbwCBum3pEXmqWPa4HbGlv0gYd5ueWyFHBBN2x-NggL8ZTe53ZpYIizZfDLDp0vfgY8Z5YyDVku_x3GElPrb2U4kpbGRwn0Tv592yobm1hOogRkdg1z8mV_oeAR5pBNL2QNZTicLmiNM6z9smiosLOvTZ7nT5UW7mJamrvuCOMGaxorOM6ntgMTtcy_UF01YD-XMgG7FpiSnlvzDPaedosa-DuTqVe0TWUOK6vlruX9agb8WYZthR4x4tD-eTecVgw7gott8F4gt1sWrmNGdRzrZud8f1_8_LNMndChm4n_sY3fA2cQojRxyAUbUS9xSGDjJsXFpcdZqCRumlY6AxwaidIuzf6UI1u0PpmfLwwOZt2MEqoKr_DTFd84ZxC0Y8-B34vB-SbY6wT8CKqD_rGlMP8XGQf3VkFgI2MHgoECIhJwN8ABSaKZfo_IVxw5XoleHfl0-Ral87-YHItZMf7Zo-CpGPQhGNFn3zzCxFfQWwinoFbJiXFbTi7ePqRZuGXlu7RnLgvKZ76dgMJ-gIJpM6ReEVJnaWwVqXX08rlGT93J4-kKRsWFWBTv5Uwd7jzLxmx86Efw8Xz21O6BnJmqiZQxhlIBXH1EGXovm8WlJYc3vF1rMs0ITqiP1PfNK35Kj4yxuIEuz6-Y_iJ_uFBunaJ5fDA-BbtvzUnLyfXSqHDI36CPaBZTnI3xLQJ8K-_M_NDxFNLbFsuOgmKowp2ULCgJjhFox6Nua7cB_ziZqyht</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fora Financial LLC</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve"> N/A</x:t>
   </x:si>
   <x:si>
-    <x:t>Software Engineering Senior Advisor</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=103&amp;ao=1110586&amp;s=58&amp;guid=0000017d035136a985cc529157229a1b&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_18ec2cf2&amp;cb=1636438194547&amp;jobListingId=1007383667451&amp;cpc=54182D2BE672C5C2&amp;jrtk=3-0-1fk1l2dsdu46k801-1fk1l2dssu1au800-9d4c55214232d9cd--6NYlbfkN0CJ4RVix5XbFvNEFGzeV6zdxykB_vlp8KSj_a_ovArNcpAUAf_1FZDHjCSGWhNpxUQMyoKTv9PM6XJueBvQ_5DfQXv_B9TQ5ZYRQ4CFNO3ggUgnV7IVmum8GxhrVOFwcxtXqXQ5sQdVkNfL_MK_SH3wf9qWbPfJnzDBPfD-S-Ev7zB7Kr5ZDZ0gXyxHnyEanqkjmtT_c8RN83ltOp4f7jy2K0pxQ9PNyjjKZK_Nv4W36dtXutjsgVX3IONol4kSyveocCnWiWCL6phRdIT_UHFB3BzCMbX45SmHuKSA4kgFUtHvTo-ta92dTuT1Kd7yeV1NazxkfpKXXB1VohHQ0QpbXuvIrVE6USwuZcyFWuFXVzsgwtzJIFdn1zsDCTqE02fmy3gpE5ztXlWHKDzaCJzxBdnF3pH9jByAT09KbUmSDqjkiBbmgfS4_xOZsqq7gWFyRL8nSDLuM577suYarkgxS91ngALFsYxcMJJ0OrdNaLdxRpOwEbCkoGZ_hBoWpCPeYud6hYFdN4THNfz4ABdIkyPFFLug9loodopajqLyA5jbZ21Jr-GS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DirectSourcePRO</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Contract</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Director of Engineering</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=104&amp;ao=1110586&amp;s=58&amp;guid=0000017d035136a985cc529157229a1b&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_c72844df&amp;cb=1636438194551&amp;jobListingId=1007324253730&amp;cpc=F7BD8DA794B5A532&amp;jrtk=3-0-1fk1l2dsdu46k801-1fk1l2dssu1au800-117d2c3d57339250--6NYlbfkN0CZjhvTnxks3zwjl9aG4M95ujhchPY6uJ5pIT_-TAyNWwWzAceZ7wwXdFj0kTHzfmG28fsS-5oi_K3xh9W0FUu0WxvJZZjBiTSyRSMOCQDnQCk9cELNatRbo6vOYcUSNivqRjZqrtAJUxJbp81YPjzFBR3Vy9WJpmIcNOUfzGLGKTHuc4JV4AY622YKdSv7sW87e1A4SAlaiAUCtJCux7PAUT9Zx3Gd4vTfDPtGq6WOeM5VXlwUpVrp7k8gJbZokPnmRjI6wYuvwgXsP1HRMb7ZE2_ZHTVHhRr1JZFKKt3c6XUuLbZQx5xqVfK1UUY96H8mi165CYSqVhUImv4uJ8KdItAzmQhl6SU8ForLhPs4Y6ba4LLeX8MPRqi9vDSrwthfAd0-WoKvUhG4BDFWnOVxqjgKWhFUaQt7L8iYLNKr3QzVWG5zyW4c0ug46xXPmlc%3D</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Torc Robotics</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Manager of Authentication, Authorization and Directory Services Engineering</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=105&amp;ao=1110586&amp;s=58&amp;guid=0000017d035136a985cc529157229a1b&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_ed728193&amp;cb=1636438194550&amp;jobListingId=1007372201346&amp;cpc=AED165184C5D3F86&amp;jrtk=3-0-1fk1l2dsdu46k801-1fk1l2dssu1au800-dc314448be7afab2--6NYlbfkN0Bvyxp-5kT5PI0anTaEYoEkcOlTMlp7z8iufLqgdrGl7gYuoiHU3tYNGHMONxq_AeZO4OER2IvEobvuBMmLvTMdPHaqt_M3Z8HU1rvkkn6uky3pM1-5Fegz0fHiXXwISWhe_6ig_XHv3FygcCR246BYBcjYBmCWve4vG5L98h7NSg9Z8AXV2fljZm2HH2b6JsEJUg6wEwBOEkKD8LocGPxXBXj99yYjeUjpO5HSk42fhnFqiMfJW5YTD3pxe_Jg48gUe4puvnBUw00ieKLPEglnZDUA35ymRV16Z_6tl3WXiZLETOJsjEvRZiQcGqixPh5RZXreNDjnG3gIbPitmX98P5vs_6h5KcBT41fBX6PtvBEGLjzoBnPRfH3WlqVJrkDY_VLnZGafcPkO0VEf9I54bOB4V6pwhvV0Lso_AgrseQOh1YU_URopnqQTqf2nfA9YK93NenHm47nbIZPslH79_-U3qjE-dAowJSFiHvcKx2XvaV6FVNHIRqhuy25NvIXIL6D_PPcxEmdYW1I8Cz7jJuW-d2ZT4J6NL9c5KmEUNQ%3D%3D</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Charles Schwab</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Senior Software Engineer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=106&amp;ao=1110586&amp;s=58&amp;guid=0000017d035136a985cc529157229a1b&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_33f10840&amp;cb=1636438194553&amp;jobListingId=1007005710927&amp;cpc=8D2B7435C06A1689&amp;jrtk=3-0-1fk1l2dsdu46k801-1fk1l2dssu1au800-4b0ba72bd5eda6b2--6NYlbfkN0ANu19da-khu0iE32scipL9wT-xpBwyDcuU4ZPgRtzex03MFjMfkX--eeFms6NZVrs2rHNcJYzoC09f83WgQfaqKZJVl2aEJhVHggNpzkn_xlqMzH7Q_fMiPin6j6MFNu6N7qq4NikS_AWIPtdVY9pnJwi2GRJshGCC_Ac86c5hxvFX1aw7F3svhklSBAjzOUsR2QMOPN75sP89lI8Uov-OkIO-G9_dDCQGK35sJw5sLhBh-09scDoFGvYmOvcfMPyt5CiBuPwgFb6LAt6X56KKb-zNnZUUNbB_0P8b7UvZYHYxl5vnPobtE8ab5qEatoRoC3CTmC0jE2eddUDEl7YPSs89lR19TlE5R1dc3sZXBrwS_8w8a7xrx0quycidlpQh8QCe7agXWjv9t7MjZcyaK3eHtvRlh9Z16WR2gEicETcettbgAs3TTRyoeG25j8vNlWb0CV0Yualys6Q9PRSIyx4ZxGa2mNOWSWbKSxQHgd3uBBPkZLelqq8MjIHTWMA%3D</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Skyways</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Manor, TX</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Engineering Lead (Industrial IoT)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=107&amp;ao=1110586&amp;s=58&amp;guid=0000017d035136a985cc529157229a1b&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_aae554ef&amp;cb=1636438194553&amp;jobListingId=1007420222584&amp;cpc=6FDD437F7834ACD3&amp;jrtk=3-0-1fk1l2dsdu46k801-1fk1l2dssu1au800-0693945a03b7b83f--6NYlbfkN0BQZmpL80JLCwCdcvt_aNRBiSGH66qw9sbmu-4MW8dYCAa7F8ejXQOcD4KiFARq31r5AskyX25i-W0hSKaKZvlU7mL6vf1EVW4Er8n5ZOB7G3a_AdEonBFkwiDAeVg3mrJej9KpKGYA_zbaUzea7BfMGKLrRXfFnbX6HblCw5Hq8pZgFVnmfcxarRzLpDIfq6ay3OJYvW0RIX9ZyA_ru0JI-58g8QkY8gtVrV6dCNAIl4GIXH8etMTtO-uaQdyDs9n7V0MK4eEMj53Xo4qrJaAA5plRPF2cTHLyQr7RzE0y4tc1-5waXd9TtSRd5-5VyxehHiT_wJejl-0aaTao0ndCMZ1jUIaRxm3Xzud5yMZOSC3zB5CAE59hMcpUrggz9aUBknctj36fzAC_MC5S_SnLrVt5ZXi7sLOBE5m1c8GVRKzIxX8yEPxMeUvzgCfDHxqO_H-5epv4RVUpQnCSyN7kek9BT9EX0JQj7YCrx6chqwgT1SvuzTAX</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ZimZee Recruiting</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Sr Manager, Software Engineering</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=108&amp;ao=1110586&amp;s=58&amp;guid=0000017d035136a985cc529157229a1b&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_aa561c80&amp;cb=1636438194552&amp;jobListingId=1007354458428&amp;cpc=D7FE8E303655E3F3&amp;jrtk=3-0-1fk1l2dsdu46k801-1fk1l2dssu1au800-7bc912fa127fe2bf--6NYlbfkN0Bvyxp-5kT5PI0anTaEYoEkcOlTMlp7z8iufLqgdrGl7itwnSg21KHIOtuVoj_q9GhqyMFGBT2_Z_dsgjYLVBUVlmQeQvDPVZz0Mrohfw62mOoT58RI5ByIjEnvxxJwefZZ3XTZi3Z1ZprfW-hsScmFEANphZuxCmo5tvwIKWVvwWJU3QMUUOQ-jHbaX2K2BlFzVoFYfOgjFWWwEXdK5iXWvvrGldemhto8_PC0aBcVnvUr46nEH4PusKavZC1rk_UH-G0RgpFQYnLIHrTns1A89OBPBnyjxvSiiwH8kPpD9zdrs7F4HxijOfE0yZMH06zRBOhsLcPzSZTeIEiYuoMpE1Ml_V5mw2jKNlDZ_LS05G03oluvaF3igZzzjAEULEqEiT9uXUva2YF-Bdnm11GKGrI-OSGQHUtUYAt_zC6FtktD8RZXRrCMFwGySopA2vrAgx5DE8XzDjm7_eFWlX09SufeSyMwFl_EXajuIGMqCAGtd2Aq5ENl_BFO1RInrzb5_0NnqcX6i_BhQ1b_fVW-j3Og9mws5rg8Op6kkyUjvA%3D%3D</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Manager, Software Engineering</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=109&amp;ao=1110586&amp;s=58&amp;guid=0000017d035136a985cc529157229a1b&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_8db74c84&amp;cb=1636438194555&amp;jobListingId=1007352307668&amp;cpc=70E6D4E49C80165A&amp;jrtk=3-0-1fk1l2dsdu46k801-1fk1l2dssu1au800-0aae5396c7d9c5e9--6NYlbfkN0CiRNM7CVr8YueLFKlzwbFWI0o7IjV438l4sVrvKZ0flkywQJjHRBleObb6D711MblzcbPJILA7DbaiMpvVPVNXVKdscBuUdls43BQlbviByGaQvJxmdCJmiGoEoSETFAcXKD9y7FSGw1N6ByKMldrbEnkm997vRtC9gHayGMdYKHfJjXX_2puSQAkwQwpTJJQ0nKyhKTR49WAs9XU5uw75PKWEKYUQhzuWe44lvJNx7-7GzVslpcQUcsy7E_SGzXGSG2aOiOYqkh84CehAE3XyEvAzzeE3Cpk1VoArvrRy2tdhMFPYKxS-fT8HRS8_wJXTWsjpRTP4M69QX1o0zFUQPXLSwE6vdULRi1W468cIom0-fvLAQG8sis25b_SCFyYhoNaba0mSIWhiD8zwFsge_Mj5RG3RhUUCrPV4l33KUeTfp9dzD1CBQGOhgvhrLxWdWKmN9bU5NGJYGBfN2fjEgPb95PqanVUhU6k4PC8nFG128uGURLrxpz2j7oEA3drdGBlEeaphAA%3D%3D</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Indeed</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Senior Manager, Software Engineering</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=110&amp;ao=1110586&amp;s=58&amp;guid=0000017d035136a985cc529157229a1b&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_f699abe8&amp;cb=1636438194556&amp;jobListingId=1007380632329&amp;cpc=56632219D727AB75&amp;jrtk=3-0-1fk1l2dsdu46k801-1fk1l2dssu1au800-4d221059ec140963--6NYlbfkN0CiRNM7CVr8YueLFKlzwbFWI0o7IjV438l4sVrvKZ0flkywQJjHRBleObb6D711Mblo1WehR2exmQCVp5hjPYq5KZLOvFjOHQJEl3wTL0ENM5TfJRcmM-dS6Cv6SDRlPEX3wGyEKQsg8IsQRN5ezc_9rc0AIh1fkTQ6tQLcq3SqWK5HH6molRVQJ3ud8ANbyv27xoso7pPB9pHbCz-2bRDBrCTCun9bdAxgNuto7ajxXDLSA_1ldBeWmCuBcSfMZdWrDs-4PWTGX2maIwGsE2PRm6cL2e_FFdL2my6vRwJTS3K9sZi7fA9fSgSsKRn3EdPyBEJ_oQO_U1vs6tN3bpbtIAsrLXk_1dy8oMyJxsyXEZ7wRPxNSYOgeQwlOjHNfAnuDL53MKGRX956UXi5g9Tcs-Shmvikfvx-aJN8k09XLtJEXsFBv-lM18KJzqCor2y49aOUsGgMGh5O7zUF8sanuOHEsgIyHZp6WXFQJLGzFwt9IFqfNR-Vh3BnSNSLQFS6cJWESj1czQ%3D%3D</x:t>
+    <x:t>Established in 2008, we support small businesses in need of financing to sustain or grow their enter...</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -469,7 +490,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="2" spans="1:5">
+    <x:row r="2" spans="1:6">
       <x:c r="A2" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -485,44 +506,53 @@
       <x:c r="E2" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:5">
+      <x:c r="F2" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6">
       <x:c r="A3" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:5">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6">
       <x:c r="A4" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:5">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6">
       <x:c r="A5" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
         <x:v>14</x:v>
@@ -534,12 +564,15 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:5">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6">
       <x:c r="A6" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
         <x:v>17</x:v>
@@ -551,10 +584,13 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:5">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6">
       <x:c r="A7" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
@@ -565,13 +601,16 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="E7" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:5">
+    </x:row>
+    <x:row r="8" spans="1:6">
       <x:c r="A8" s="0" t="s">
         <x:v>23</x:v>
       </x:c>
@@ -584,47 +623,71 @@
       <x:c r="D8" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
-    </x:row>
-    <x:row r="9" spans="1:5">
+      <x:c r="E8" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:6">
       <x:c r="A9" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:6">
+      <x:c r="A10" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:6">
+      <x:c r="A11" s="0" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="C9" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="D9" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:5">
-      <x:c r="A10" s="0" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="B10" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="C10" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="D10" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:5">
-      <x:c r="A11" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
         <x:v>3</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="F11" s="0" t="s">
+        <x:v>38</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Left off on ZipRecruiter Workflow Write Range activities
</commit_message>
<xml_diff>
--- a/Job Hunter/JHClientTarget.xlsx
+++ b/Job Hunter/JHClientTarget.xlsx
@@ -14,126 +14,137 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
-  <x:si>
-    <x:t>Senior Accountant</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=101&amp;ao=1110586&amp;s=58&amp;guid=0000017d06c3e4d285a10d0346a6b2e4&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F2F6F181172E0D6290C2D13E89699FD&amp;ea=1&amp;cs=1_9489ae42&amp;cb=1636496041676&amp;jobListingId=1007332495127&amp;cpc=FB91BA2009EB6168&amp;jrtk=3-0-1fk3c7p96u49i801-1fk3c7p9ru25n800-813adafdebc0e24e--6NYlbfkN0CFheh7eSUSHEwDr_W6ox7XeCFcxwMCK__nsBuF72--9iLa5ffHcde-fUzwP2p0dU6sHaEN_fyln_BLwf_1lFfYoEQkNRFtBY_4vr_CHOrJvodoK7Z_MUciXE1A5fdQ-MCDAD2WmNGM9dTDO-I67e0BfJtdU0nn0bZLp55N1xcy_qQcknKAP9S0JVuupXhSU5buWs5b-Jd4Ajyq1HilTQ9JaXCmn4iCyBzzz-PW1FaMfU66x11j4VkswavN6d-vc0c8QtKedrjn36gXPysNdjNqXumAy0RTqmkgX0LLX0Rbn0MgqVi8y174GST7s7J34iyTyMf1H4GhHHg7hiSOKuOpKLA2pC7v-k0G7eu4BmVRNya_6tgv6_TxCUK48sPYdzw-wLW3avEkWA5QdSkDCXa-8MBxBEmKw5HYfv8X02KO_86YF54PlHdq21Gp0kUBF8zQmBvUPcgVbIwXu1DAQ67xQXC8pjind4ln1FE2eSREfScsKxYCPjN5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Diversified Real Estate Company</x:t>
-  </x:si>
-  <x:si>
-    <x:t>New York, NY</x:t>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+  <x:si>
+    <x:t>Process Engineer (Seminicondutor)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=101&amp;ao=1110586&amp;s=58&amp;guid=0000017d10b58b94b5a2c646a3c53d63&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_6c7bce4a&amp;cb=1636662873437&amp;jobListingId=1007423340600&amp;cpc=23D1D7905F5E0EF7&amp;jrtk=3-0-1fk8bb2up3of6001-1fk8bb2vdu2f1800-6eff60079a12472d--6NYlbfkN0D0_CP4C0npbIk-x0XKq0zU8RDkvyqf0CxCWzZ3t29hIkPUgM1bzmBy31Yf9bGv0JZ0KFVSPTREYz7B9ZQRBPlfoe9u2iTQiZcDG1ix389M_InkddXVYzLKUM2v2PZEelkEGwCUO7x5bwRALlGUXXfcHM8qc7Uz5UFgZUwn7MCuaWb7OK8VZllUfZZoDRS9vU3aOQFYFAqp4HdlEooTXUHDh8ZIxymOFuZOEsNjlu69tPtPTVugRgarfp7SUmj3pkGXE66czhfaSc4knBMBbx1k51JoNOg7fOBSonMrp8fuv5agdZGqDP6NRaV0dyD31n74A7e3Xlp6Nm8z4LEbeGa1fp9dReZ_jImsC37c0oxmUDgTqLEkqefa1ZNrSkXVF4sHgENtgHLsAVYoljUEQF1NoA7wSSuHxSHUUWKdjTGz18IykEosZ1CXOygSr3ekItYf6dU_CNjTIIyp3bgyXnIcAAzrTLwuxL3ENR_fR-yunUysU8f0hF_8LsagddVfr-U%3D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Siconnex America</x:t>
+  </x:si>
+  <x:si>
+    <x:t>United States</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve"> Full-time</x:t>
   </x:si>
   <x:si>
-    <x:t>We are seeking a bright individual who can assist Controllers on various accounting and investment p...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Staff Accountant/Senior Accountant</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=102&amp;ao=1110586&amp;s=58&amp;guid=0000017d06c3e4d285a10d0346a6b2e4&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F2F6F181172E0D6290C2D13E89699FD&amp;ea=1&amp;cs=1_a79df394&amp;cb=1636496041676&amp;jobListingId=1007165460313&amp;cpc=AE9297225A38C224&amp;jrtk=3-0-1fk3c7p96u49i801-1fk3c7p9ru25n800-fd094cdc4ea10606--6NYlbfkN0CsiqsuAtvdWzPb4b_7B96DIrhySPzdv4FG7XsbZH1FPtDztzrDmbS4BNMha0xZ_qn6gPXZSI82rSnA3pJ7n0waD8uH5tw7SFJVfGR3lWzhwEJhMMLgKQlybaA2_q7THK278rx0GDQSsTRpatwfz7uKSfZ7sK7JbA3p_3DchLsugDILeCDgwpi_StoW4gyq8WbyEvrs3x-vb5oRe49QNkyHnBMWU21GlkgzSyLx3HLSMmWUZWvayYkl_FGQPaLI2sMLZ7FJZ_Q-O0ReltNMzIN4T8nU2_5yJYel4CWaEc9m3xunMP6ud98EkFdpB2atuaQvXNJgea4AKQNi7RBY6CVxNQ3bVZ7jmPn3X0_NfA-fSxvlsH7GGRKM3G2of53rmRsgqzUmDfqZJ-KOymHAjDlRA3xx1Gf1yCkjdb61OGladmJh5jdPYguXST2NHFbhoc85pJJAaSqtItpDi0EZk0t1tT9r6EHfNrYhoW-LSscLp4-HvsGm8G7vGao9RJGY45vZvNKlwY5ghA%3D%3D</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hoberman &amp; Lesser LLP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hoberman &amp; Lesser is a mid-size Certified Public Accounting and Advisory firm, located in New York C...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Semi-Senior Accountant (Experience Required)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=103&amp;ao=1110586&amp;s=58&amp;guid=0000017d06c3e4d285a10d0346a6b2e4&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F2F6F181172E0D6290C2D13E89699FD&amp;ea=1&amp;cs=1_2da59344&amp;cb=1636496041677&amp;jobListingId=1007377411152&amp;cpc=A50357DDA226FF0F&amp;jrtk=3-0-1fk3c7p96u49i801-1fk3c7p9ru25n800-a94848b4b7fee52a--6NYlbfkN0CtwOkgDuej6vPfWODMxjOIyNEohQmdYMppGq8y8dOpBqaQGVU4tVOVpluzlhQ8N9LO-I6z2xgv1D197IRt-TjPdzURxQSNYf4zbzEx4vIeIBcdol_xYzrCecFx5sL2vIV81WENKyi9tqrsmGoj99V347IKmefJvbTUkrg7NhamIsO-oF1wS04SJ03UyZMVQbO6AOa7pg_t5pXaI5-gHywrEokmrkKIbmLOoN9oEYJDWOM5hDdnVANqWEgRqPvbTTa02efbk_WOIUiz64T34mhYA_JADJ56Q8ME7NYKQeM2xhaC-AmE5HCLkd5dgMrn-fWOeEkBdRAL-KRzFZ4-7gWmnHg2lzKPRzTUwbpuw0nVxtwhcfWaeLlEETfqBjVsZ5ckx8tzAEnVo_QdUydJm_W-LOblpwS8nx-jXO7pzN2wJC1yxE76Xgip_Bubx7i4IPiN0iWSAVh_J9fFAEZA_OIVQ_YFM2vUId6HYaqo8lSPRR9HxvPkaFuYdar9ZjfAz_SPl3woQ8GewvMyeRKU0A-0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Raines &amp; Fischer LLP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Our firm seeks an experienced Semi-Senior Accountant with a drive to interact with clients and learn...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=104&amp;ao=1110586&amp;s=58&amp;guid=0000017d06c3e4d285a10d0346a6b2e4&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F2F6F181172E0D6290C2D13E89699FD&amp;ea=1&amp;cs=1_a2876139&amp;cb=1636496041678&amp;jobListingId=1006936933899&amp;cpc=241359978B7FCDEB&amp;jrtk=3-0-1fk3c7p96u49i801-1fk3c7p9ru25n800-6399f9587839b797--6NYlbfkN0DXIqEcRagNjM2D6V3zaAir9KeCGU1qEKArEmDBSQxJZKbydGVUJc8eWrhfTOu0fQHkso6us9haOYM65fEiSkTBrQAAebCYVJQqrT5-TfXHugi_6PP0CP9Yk2F7EE8uiTNKEwew6tAjpFWrtSXbd3UjMWcTspdova90dfwm9EGByKs4R1Vz_kQYU-hXBJFDHBI3y6XVWlMT-FzPHhcvH5L6lcamy0YG4g2JeEfSed4L4EwBDh9iuhdL3gV_XtAJTJgPQEW4nEWQldAMJkTThENXCFREBNJMmMGLEGI5f5VjUz50WZElB49D0d3M_zGI1X9OJGJTZfNwk7EJFMeH3ka09EP5IlPiXQs7bFKZMTufSU6oXWl4m_8RqHURu9sXPY8JOQGlUNWTSVSUbQupVIqr04GhcWB6Ixk75aakmocRiKQchq-bYzLXhcoUb0xuuLkDflFDtgbzIhvJAUExB_qWndPGBF-ekLeNEEYVJQIE59LPfdbrK4Pm</x:t>
-  </x:si>
-  <x:si>
-    <x:t>New York Design Architects, LLP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IMMEDIATEProminent 25 year old Tribeca Architectural firm seeks experienced Senior Accountant to con...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=105&amp;ao=1110586&amp;s=58&amp;guid=0000017d06c3e4d285a10d0346a6b2e4&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F2F6F181172E0D6290C2D13E89699FD&amp;ea=1&amp;cs=1_d999abf0&amp;cb=1636496041679&amp;jobListingId=1007401869275&amp;cpc=F4CC4721A073827F&amp;jrtk=3-0-1fk3c7p96u49i801-1fk3c7p9ru25n800-b7442ae82af528f7--6NYlbfkN0DAwgduWqBP7ymGN-lTADpinz2i-23XbRAyg5ywqS-MDYi_s7Thtk4lX7i5GAqNpXenlvJENKGQs6YdvXdI0JXj3C9Pv9Jf9N9UZaon4gyRN445XQP_OBYAuEnCAaaY8JdGqvY_ojI81lyMfn3YwUUaQbVXU4kfX1S4sqrSmIE-1umlzCB1LHoJ8rl7-LqIrSgtlrg45IafqtNOvJ4w2MVzF4I-k6CkNFOUPt2X8RIq2O3KBF03G8I0YMZqS2mT9p5nwRfIMR3g6G3YluDNa29i5I_qG8BCH_6a5teqzu6zsxBACLsFxXZ2C5ovRA_S07OR6EPASoNU5omzs9zn2Z5ZCAmQ7Cf0jsGjNpfp8E48uUvwqWR1YUX5sGSVZ_Crs3U3NliT0Xi0AoTU_p2soq5jLnh4yh-L3A6d9_hMwAyJ0_JvzDjz3qHkAWMRUPky7blkSLF220RD7Xn2e7uj9h9IcvMW5yWfmxis7HWYT12yyHiG5EQ3cgOW</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Toscano Clements Taylor</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Staff Accountant Associate</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=106&amp;ao=1110586&amp;s=58&amp;guid=0000017d06c3e4d285a10d0346a6b2e4&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F2F6F181172E0D6290C2D13E89699FD&amp;ea=1&amp;cs=1_7f6161f2&amp;cb=1636496041679&amp;jobListingId=1007246985322&amp;cpc=B3B142CD6B71FD88&amp;jrtk=3-0-1fk3c7p96u49i801-1fk3c7p9ru25n800-0df76712f5386efc--6NYlbfkN0Dl8IMvTlUpyY0fNxFFsmnRGIkWh_m6VxgQLP5Pfft0j792K-wCd8TjtNXFufRtbOXvp8L4Iivi4t6jeY4rqErxOuu_sNqmEJ043nHL8YepJZY5aK5jtVL885a5FKNqO8tjXOkb8AavjXank3WKoAS4kmzRrFflP80oAd3dbU1cE0xoAW4A2SxteEd8CiijqSxOhP2ogmUnATV3iI9v1JZFFzSevUehTyUT6zijg8xksBefS3FYV8EPEz61PG8SxO7ywlJdeOQKal4S6C0lmIRRP0Pjza8WZamLVScl8wHyxfKP-dCkIZPpuuT0ouYh_OWCioUiFDW0s_gqcqAovlLSI6NW8aUa0Nx2V8RhpmuQwQtY2RN8XyIpIeBMW3pYcz5_0L0yhoNv1wnbGbXbTWqTcGznmSCWthXKlTfvPx_UpNg58CJcyb1fcTw7Vy16K84VStewxmMY7-Nlt6l9osptwZikHAcq8H5D4wcmGcDaTfDWAFn4UUaUys5xdFXKFLMzZtrZzo-DZaI5svvO-ec-CG2a3d9wPGVuMc69mn6SVWDiM8Z6OTcy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>OTC Markets Group Inc</x:t>
-  </x:si>
-  <x:si>
-    <x:t>OTC Markets Group Inc., operator of premier US financial marketplaces, is seeking a Staff Accountant...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Staff Accountant - NY, NY</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=107&amp;ao=1110586&amp;s=58&amp;guid=0000017d06c3e4d285a10d0346a6b2e4&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F2F6F181172E0D6290C2D13E89699FD&amp;cs=1_61620436&amp;cb=1636496041678&amp;jobListingId=1007399629954&amp;cpc=F5D43257E3E73E36&amp;jrtk=3-0-1fk3c7p96u49i801-1fk3c7p9ru25n800-861dbb5ff383c8e7--6NYlbfkN0DN0uKknIRIeHRZyobcf3FRiQlpXuSIu20Fm8rTPpuaEScs5ILohoWoCsyWJ4d6sf_KW_vToU7N4fR9jkXdWAhk2qns99GxRgAm4Ncz03_i_D5D648u7H6didrRuJFofLtP1wfWe1p7cQ8WbTdBVP8i9vyKgc7LHeoWhcb5f5OjABXhO-PoBwd04YHk2YeyJBH5sP-ZBypBqk69yxADBexPUvUOZFn32V5hddiYXUTqucmL3JHu8HOUEeQ3BuNDIwIsdWSxSI-h2RMwnDPVkjgJDa2IDzmCxVF-nE0PtJkjuT6Ec-jv6e_aen4rRaKKscLyreBFpXZIt5frj5Si1wwkHe2VCK3E6rzI7kLC4hKAIZoXODU8uY5O4AxhZ40KyldPHtjCxS1sdYr58OmN3kZT-bOroPG7ZS4Ow5VSF0gvvxOpolPOgiFP-7laD5eO8cCplUf9ssOitnryPir2uXTvRsdwtPtmeXKnpT0TtzqsiWOcs9msbGpiH63im6GTr33Uufb4bSbFF-DQGu9sVTSCqyDzXACGrX3_wz7r-DOg5C_o6929tWHRnZRbT3WrlC5rolyz6EzApPYI__JhZKJEBZQpb3rwX4zZc8c_3bVlZ5VFxIjdgqcYdHH6HBPTH__ZEDIDLv9XTNLNG2aQr3pnPg3Gy8peE-MLstZ8lcTJlSYp7W-tMYQB17GAcoSTJABYo7wRkXt1SqVDMpMkOZ3LHDtfRYyFZW7oYEhtNekfHST4csWnWfQ505Xa4noKDvhHgPHbzSgvKCyFiL0JGRMp</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Your Part-Time Controller, LLC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Overview:
-Either a Full-Time or Part-Time Opportunity
-Your Part-Time Controller works with nonprofi...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Staff Accountant</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=108&amp;ao=1110586&amp;s=58&amp;guid=0000017d06c3e4d285a10d0346a6b2e4&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F2F6F181172E0D6290C2D13E89699FD&amp;ea=1&amp;cs=1_3408bc06&amp;cb=1636496041681&amp;jobListingId=1007363832948&amp;cpc=B6E9EE473EF69035&amp;jrtk=3-0-1fk3c7p96u49i801-1fk3c7p9ru25n800-886b0e4851fc04e8--6NYlbfkN0Cy6Y0fLVKZlaLIH3HmWBB-umnKJBe35kIsW8Zj8Ud66Iy5GzJSobzI_R7kfD5BXSKa2ebF0B1PRkB4zvGh4nTs1yvmebXlDifZ2zfZmYk1SsmHla3OxBDOtTljSod5rDO4aH8LccOirqFBiJo8teYdkOshsBtVFE1GHhpocFVgLExkLbCoZrYp9LqZ-T8Nd6LlYtdls0rueEndPTa1LL39pjYIP1G4naNC8vh31ZKEKjE06WfqeDX_Zyhsv3NBbhAQMlpPRz3yYJHpLu5vsvb2_SLnJEegSKYgbcdEQ1DUyCdiFvVFdBrbqgvRhhnN2I8Xv3gGsFeWAQOhpdGjYxTIym-D4-5T7JQKYPKs8Htnx6_ku-VTZnfgdxcFUWpaCFSwPGX4OBKQ_O26Pk44zqbBwGEV0A2rMh3qwdg-bwSM4u6wWxISk2CPIvH2eT2jXuIRaV05iw7yvXERl5PMCkwExaOs4C4mZ82cSl8NuPHhS3xKQBPbo2NMX-GyYvqWRjM%3D</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Biz2Credit Inc</x:t>
-  </x:si>
-  <x:si>
-    <x:t>About Us:
-Biz2Credit, a Series B ($52M) financial technology company founded in 2007, provides fundi...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Senior Financial Accountants/Analysts</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=109&amp;ao=1110586&amp;s=58&amp;guid=0000017d06c3e4d285a10d0346a6b2e4&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F2F6F181172E0D6290C2D13E89699FD&amp;ea=1&amp;cs=1_ed62c637&amp;cb=1636496041682&amp;jobListingId=1007403100390&amp;cpc=90C4CD7F4113B630&amp;jrtk=3-0-1fk3c7p96u49i801-1fk3c7p9ru25n800-c0033c647f66c986--6NYlbfkN0BdX3W3WyFVN-ulM4iCZnMv8qZviPHHsAQc8kaRA1cR_dlcOeKDcEnDnW3QqNbPVkcEHwI252y3V0nuy5NmxzzBI7hIQK1KXoWURrcZsr1i-elYoBpIfjRgGahKtZSqqsTsrKG13muNqcOC9M7MNrzkJwUD5TkcDmJtn592F1Qdy9H8nftajfE8JRpWeXZ5OppH2ESCxNNV-BoHelovaz7IMccVqv6nrKnQBdDq0w-14zUTq5pm5FaiKKIPap-BXxx1p8Dek9Z3o4j662kmULJvxgfrPVzVnaN-yPo_7hW7KXM9rAfHei5n9AI620UlEi2reCNgFUcs6e40B962VTtZNroIU8CnLILpAZVwkmeQn82avowGk9HP4F7HsLpepPgO7B5m1vhenjKs_YJB7xIWlL_bOPFVv08oouACdDQr8a_9IaB9DdkHPIWQ5sbFpfFvbFiusgIIh68FnjrinshOhM7JNETxf61A2DGaOfL-Z_nInn2plEI6PlcrnV2cdljKfMVn9sBE5NqYhTXVuLe-</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Access Staffing LLC</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Senior Financial Accountants/Analysts$130k + Bonus(Hybrid Position)Two of our largest global and exp...</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=110&amp;ao=1110586&amp;s=58&amp;guid=0000017d06c3e4d285a10d0346a6b2e4&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=8F2F6F181172E0D6290C2D13E89699FD&amp;ea=1&amp;cs=1_51acfa2a&amp;cb=1636496041685&amp;jobListingId=1007407883193&amp;cpc=0AE43CF55DD5119E&amp;jrtk=3-0-1fk3c7p96u49i801-1fk3c7p9ru25n800-b58bd8b0623b94aa--6NYlbfkN0AVmeVdBxbwCBum3pEXmqWPa4HbGlv0gYd5ueWyFHBBN2x-NggL8ZTe53ZpYIizZfDLDp0vfgY8Z5YyDVku_x3GElPrb2U4kpbGRwn0Tv592yobm1hOogRkdg1z8mV_oeAR5pBNL2QNZTicLmiNM6z9smiosLOvTZ7nT5UW7mJamrvuCOMGaxorOM6ntgMTtcy_UF01YD-XMgG7FpiSnlvzDPaedosa-DuTqVe0TWUOK6vlruX9agb8WYZthR4x4tD-eTecVgw7gott8F4gt1sWrmNGdRzrZud8f1_8_LNMndChm4n_sY3fA2cQojRxyAUbUS9xSGDjJsXFpcdZqCRumlY6AxwaidIuzf6UI1u0PpmfLwwOZt2MEqoKr_DTFd84ZxC0Y8-B34vB-SbY6wT8CKqD_rGlMP8XGQf3VkFgI2MHgoECIhJwN8ABSaKZfo_IVxw5XoleHfl0-Ral87-YHItZMf7Zo-CpGPQhGNFn3zzCxFfQWwinoFbJiXFbTi7ePqRZuGXlu7RnLgvKZ76dgMJ-gIJpM6ReEVJnaWwVqXX08rlGT93J4-kKRsWFWBTv5Uwd7jzLxmx86Efw8Xz21O6BnJmqiZQxhlIBXH1EGXovm8WlJYc3vF1rMs0ITqiP1PfNK35Kj4yxuIEuz6-Y_iJ_uFBunaJ5fDA-BbtvzUnLyfXSqHDI36CPaBZTnI3xLQJ8K-_M_NDxFNLbFsuOgmKowp2ULCgJjhFox6Nua7cB_ziZqyht</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Fora Financial LLC</x:t>
+    <x:t>Siconnex – Expertise from Austria applied around the World as a leading equipment manufacturer for t...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Analog IC Design Engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=102&amp;ao=1110586&amp;s=58&amp;guid=0000017d10b58b94b5a2c646a3c53d63&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_8f7fd56c&amp;cb=1636662873435&amp;jobListingId=1007418453986&amp;cpc=4D489A1B82E31BBF&amp;jrtk=3-0-1fk8bb2up3of6001-1fk8bb2vdu2f1800-61007509a62de8b9--6NYlbfkN0Bmo50VnEhsYYirJ0OOu8Fb0y9AeI6Uo6oKg4EqHIsGblqgkBctQzMQnvENdAOmY102QYp43fGGm4rUcVFXFGJpFqNE6SjXQx8A-nI2GXCf7vRsIPje5EFuH6-juhYwP19CeWVBL01PLcWng0OGZJ2E-7V6AFmIX_dvYbQxl15mPL3hYy4E2zPpsC2iAHA1WZCemi3SGZjlK_RIRzQK77s6mlZFsx1E6XctNS16haqICH9Lg7YFOByXbKeXH1DxAhvcSqvRmx4iv14CrzCRfXiRk2prqua9EvNVXeK0tpwhY81eEBx7ibvD5otRik8KgRFvuOdijjs-Y8i5_wvztAkK1hPAHpq5DRtR-pH2Z3s7pGODIZiBpdnRMgzD0XOfZjfYdcHW7e3VcSKeZwxaDia5z9lXmjS-ntP8xqg0xCNOGPrDfZW0hxlAkvAJb913iZariGQSAtfWfHafxxGEVFGA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Texas Instruments</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Texas Instruments Incorporated (TI) is a global semiconductor design and manufacturing company that ...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Equipment Engineer - APPLY NOW!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=103&amp;ao=1110586&amp;s=58&amp;guid=0000017d10b58b94b5a2c646a3c53d63&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_397b931b&amp;cb=1636662873436&amp;jobListingId=1007310809481&amp;cpc=883DC43018083D9A&amp;jrtk=3-0-1fk8bb2up3of6001-1fk8bb2vdu2f1800-1872841e48ae4257--6NYlbfkN0Bmo50VnEhsYYirJ0OOu8Fb0y9AeI6Uo6oKg4EqHIsGboLSeuaR-wvTtUTzfUxjVbp0mGfNEE9BylEJoa5eGCTF-SlHqLui38G8Co2YXZ2r0naIe8ZbGs7v10sNfFU2BfOLkUyoIUGeJnlQ3Bow2KXtMxbqm4rMKMejstRYlIkWOlo55505OYUE4pzP5rYe7j2HnvLnXIFG5QIuBzpoZk3_wSCJZtrFKZmUHiwD8CXipYXmUfoLbGST1FoCtxATRSRVzxFSy1PdBYCz7tgkCznfftcZcnPO-9Lx5UWomy2qV8IBcNNwVP-zcKU7_oL7lROTIzLSJQojgRvE9enHegS6JoAYIyXuMFhfoGwJDqXyUG3WghtiNz6nCZi1q0NntPXnEFnP_JnUZWs_nkGNJxf0MP6Gpjq3wPoGO-G17s-Zs4LIVjtMrUFWYyHJnOl71cuc2_AYypQaSg%3D%3D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Robotics Automation engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=104&amp;ao=1110586&amp;s=58&amp;guid=0000017d10b58b94b5a2c646a3c53d63&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_99bf40f6&amp;cb=1636662873439&amp;jobListingId=1007430058863&amp;cpc=3E251C7E648E8D76&amp;jrtk=3-0-1fk8bb2up3of6001-1fk8bb2vdu2f1800-faeb1b710b28c42e--6NYlbfkN0BXmJBcfPS63VHBQ4gvdbS1h1gZSZauv-fenQstXctAlIGgiULABlXHcmnNQz25swCj0EPo0_5n6aHlu2knvEavlEF7g0fV1B2AtzEXZjCvtmyKKP2Dz9kvA2VsPSzMmqhkVZWFP4K7QlaTL82LnPQkEoUOv-AvqjYGNUfcwlc_bR9dWnO_sQ-46t2I4fz9kskiGSypCFBguufAWMFSME0uLxgXhqEexxqBm2rw5tfBWHzjL-CoQShPfj_-rHqv2kf0UlTA4hXBvk_LQjc4fPtnvZ8JLxpIMXZqvxaA3HdNvZE864xZdaqVnEI4XJw5Ur5MhE5U09A5RdCaYwG_jd7k0jkzx2r4W9tPWM7skyW7dIk6nGG-xJMjAYbddv6M4UDIUPJoDqVMMHdwvAGWUXqcKVKvM4_Wjaui_PphVJn-z9QmRykGMRnGtwqo_upL0yUPBr2lXH0qsjYf284KoI4uy0KKgdbuv3xCIVYfve5yEPobFahF96g__sIvJEFf_uE%3D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Phoenix Innovations</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Flower Mound, TX</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dream the automation and build it.. come join an organization that is rapidly growing in advanced au...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Controls Engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=105&amp;ao=1110586&amp;s=58&amp;guid=0000017d10b58b94b5a2c646a3c53d63&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_b0d0ea5d&amp;cb=1636662873439&amp;jobListingId=1007429029643&amp;cpc=A938E184CF850189&amp;jrtk=3-0-1fk8bb2up3of6001-1fk8bb2vdu2f1800-916d23fd85cd54f1--6NYlbfkN0BqJjBsvJkVIRVupdyx-l7jJlkPL5nU6SVET5Mq4mDejcdzcnu2kZGUYkGj0MnsoTA_KcSE-8whlM4pLrfJtWercf34uNzcmM8pFicP-70xT--CkGbE2Gs0Aj4gdz7PT7YFaplBHppkjYp8XWb7Zh6MWuYWDemexDEcg8tUsyoV9gbzEyi6zqUa8mo5v0fZE98-qF8Tnx5shHbt-9QrgKMufqEDcIucAuqsVLM3eNaUrIHIAKiCbNvFyoisgxohbGX547p9OpxJbcn2DeCN84jyzHzGd0CFWDDle_3uOsMhIGZw2qQ9yfO8o5kAkXD09eEWZ1nNdnXeoeDn-mx8G53btI6sHi8Ijo0wNLXiCA6s8eU9Gy4GomHRyMOOtWu1X6fK7QTCX4zs2p1nmz-zFMpuuYhIjwTV6G1PyVc7nhlMdl4mB9TFSMVJNNUI-kLNIE9tJ2yZRsEuTnSrpmeHizNbYtMdddnhonxOFv9VLkDzGDpYRviwqgxfyOo2r3PrG2Yb-FuA2KnW5qDpFYgR5tNPJ2tC0xOjym4Uvo6EUI4cJOfaIH3hijYsMIMxw1EJ3m3ihtMB6ar6l0Y58WMuSrdE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>General Motors</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Arlington, TX</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve"> N/A</x:t>
   </x:si>
   <x:si>
-    <x:t>Established in 2008, we support small businesses in need of financing to sustain or grow their enter...</x:t>
+    <x:t>Automation Engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=106&amp;ao=1110586&amp;s=58&amp;guid=0000017d10b58b94b5a2c646a3c53d63&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_476ec062&amp;cb=1636662873441&amp;jobListingId=1007426777663&amp;cpc=8CDBB1EC89CF7160&amp;jrtk=3-0-1fk8bb2up3of6001-1fk8bb2vdu2f1800-b2925a9a62748c4f--6NYlbfkN0ApT6tFA4QF9s4NLwBFQFVdBAjLZKVLZNsaFTMwoZu1PrEydR_cad-mxwf7KV4h7DqFSEy178JfkLNDa1phEXcGu5k_BXI0T0Vo6WVn0_mCzJyjY6Xb-xZ6YZ-i-q8ent6sdekzsecdGG_Wz8-GFMQ5TzLzFifzkOrWAdneE37ZlsU6C9DBAoPaVvR3iSfFLzjpMKD7rnDiApTZLbTIC6eFFeBMo9UQYriyoTjRrrKQ6LVLzgjLtgjevXjgEbfHQoqBFnyBuFm6J7OOmC5vOFZvRAvOa9c3YXaxM57KLpr67ASpOCv9SyC3NR3wzx9qSA0GRis9kC7GJaYza2_yECsnf21Bv3QYrFe5VYrTRTGKpMLAfITF3tL0vzQIKDq_ef4duGO9sGCEogBt7zJyZ_KZr_1jULg2BWL_Rp20NYhiVAnQcdGp_5BN_dd3BghdoBnUXLoRehlptYkkNkdK3Qeh6xTqofZIXbj8CBF2NmVWoMVi-s8IYmJfvAEgN8yzQbQ%3D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Crimson Chemicals</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Texas</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Automation Engineer - Chemical IndustryResponsibilities: Work directly with project management to de...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Operations Engineer (Remote)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=107&amp;ao=1110586&amp;s=58&amp;guid=0000017d10b58b94b5a2c646a3c53d63&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_78f16aa9&amp;cb=1636662873441&amp;jobListingId=1007349474016&amp;cpc=AF02A54CD0F60729&amp;jrtk=3-0-1fk8bb2up3of6001-1fk8bb2vdu2f1800-ec31f96ef87dd3f2--6NYlbfkN0CHmpUCSxDYjXqLwMq9sXRhzZbRYXAhXF7CEKQIH7J0VvtJGNeI-4OLPFQDa-sAT2fC-0H9nMcj4xcKmyZJapRLy9hrmnJBVBUdy1UpAjKC0UPYwxJsdswspvbnIsLpcVAyRdgqBei_X9PrqURwM-k6U0T8bzROkGgWWe-dLZ1YUkvHslrHgB-JczpnzjtuvdnKIAXR7rNa7YI48eqePM-15KCVVg83JvutEPMM296iq-BXVFo0ybeA9uXw6_c0AkivGwYo6mK9J_tMJ5PX05zdgBehJ3-IJa6nvW5TIJGdu5T3xOFPJykpC1cH03dhEebtmIzJXWdoW3GV_IQmteSqjlU94u-EmysickWnm29bmXH9I4hy-Sn26i1IzS7PvfUk1FEZenMzWHbXSLhoMrykqEBnoVtZmL0MU49FZmtJMKmMFz8XowaaYuFQ45sgLhg%3D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Oscar Health</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JOB
+The purpose of this position is to complete independent reviews of developer proposals and capit...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Civil Engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=108&amp;ao=1110586&amp;s=58&amp;guid=0000017d10b58b94b5a2c646a3c53d63&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;cs=1_2360d8fb&amp;cb=1636662873440&amp;jobListingId=1007424393144&amp;cpc=9BAD89CD83072753&amp;jrtk=3-0-1fk8bb2up3of6001-1fk8bb2vdu2f1800-3784301de6f5c3fa--6NYlbfkN0AC6SQMfAkHCondRquBNcE2ntt1snCy3fyoZRReqai0Ock3efZYNuf6KvC8jzoHnHy5aeekgzu03CYSWpjTBfXU-752Okcj-SkfMfgkk81qzVUmrla-BruNztAWgUIbAd4UlAE1kWkolrQ54jjlLMgQDE_FfxmnQWVpxIO8R8v0ciKlAu17inOEuy5_ohNp1rrevHJ3DIozf1t4IkkSR0Qx2EWxhdxzaLqMts7cJAqLnF8Z6jrP6Bt85Ohl3qJq0g8jxVY61yjvAlYt6U0UXJKp04o6rvpo5D0YCvR8UecNMo9HbuBJUpquZcNbyYeykvAaIL_smLPILE1UAuHdln71X8m2Fkh3EjV0f0uD2ZprYlEyZfooamEftTmJQSoC_jZTN0-iab3pQrgchsCwS8zowlLhU8tkwBRQPz7HeogMGThUfdpvVXGfvG3agKa_-WLudl2VqnYlq1GUm5SCyBUOu_yqwiT_V0E9jRP1tFs5syzZP_S_ynPYp03e74ftrtfn9eJFHe-HUOHyyRf2FXLs2D_IUk4DChxTV8PkFmvWh_NUvBWhjUbWeIh_4QnGge5oN81K76C4btOcaJ-SKp_labG4RIpCvXCAfR13dR3_BqEwD6hfgLyiPMK2EUpZenDubYYyQ4Oyj9QDB_kjeJCw_w9dLFtNpbZtQCfebkKe7aSMRk-27g7raR5lm17q1dvHtbhzK86uUaYef-Kknf8SuUtoEfHXgcxrIA0oFhyRQEGRgUgTMUOqGZJLBDCtP4AkqJU-z-VGtxgXYiSGzvqBJIVSSHDFNd0qVTWgb7A4To1D0BzlAK-5mE0kPMRjJob5Gp7akvhkEP3iS0cb_1lvSX76dquXge6G2MLu5TX9TjwLTUjv7ESP6qghT6BgGGRWX80M_i5I0_rvcxEq-la_5MmBoknYJ1Qkdflw82yUctE-FUczMxCDQ_7JGX0JsuTk5XAaFjpsWAPy6D5Sa7PVbOB3YCIB1AG5z56cNV4ZUnSP-E5vGeWvttFnWtXwSTjIE7NZz7uSDT2-U9Dn1M0Bil74c4dNQIJ3ZKDkGBYD0w%3D%3D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>City of DeSoto</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Desoto, TX</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hi, we're Oscar. We're hiring an Operations Engineer to join our Insurance Operations team.
+Oscar i...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Medical Device Manufacturing Engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=109&amp;ao=1110586&amp;s=58&amp;guid=0000017d10b58b94b5a2c646a3c53d63&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_d2b9b0e9&amp;cb=1636662873442&amp;jobListingId=1007403878413&amp;cpc=E773D000C9BC26FA&amp;jrtk=3-0-1fk8bb2up3of6001-1fk8bb2vdu2f1800-855f6c25ec112de5--6NYlbfkN0AmHEW7ezYoz3qdHICrbgqPAbIqeCN9Klocv_B1s1YAxfzgkXLMblpaM3-0Mjcj2rnXp8qgOC9TPp52LVpDiJis2b7Aohg0xhZwuLcsl5Nmhga7teTMzrR2CFK3kzta0YLhGtTK6d_9pZMzlYB1WXqWIffkcRW6LZSovonu6bf_Cup-KlMyYYRfhU16ami2y17svGwwW0c3jxgsaQEn1maNtoNW8wROJxUTtfr7DUikkK2PE1eV22mZkdKPyZMAtDrjMkRNj2l1QdmbS0WSixoBc_dq3B-bHZHZOEu9ptJb60N66R05dkmedSfICx2YY2AiYgquYc-D0OkDlliFWFpbo-22E57yudwY5SjSlnqyb5DmT1Uifz9fJHB41EKn2vuJ9H3l7vdNR8RqTTrgfJYnhkVTkIXbP3CSZBHFHYdtCZozUj6GVQ8H8FI-KDu-1lNxIWEpBXUfQtmm9RiyvNmqBf2FwBvboRIgflSmMb8kKODiVhGjAhSDGLr4TzNEHW-ln2fhZIlMNg%3D%3D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Griffin Global Systems</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Title: Product Definition EngineerWurth Electronics and the PDE/SPM Team: Würth Elektronik, part of ...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Radio Frequency Engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.glassdoor.com/partner/jobListing.htm?pos=110&amp;ao=1110586&amp;s=58&amp;guid=0000017d10b58b94b5a2c646a3c53d63&amp;src=GD_JOB_AD&amp;t=SR&amp;vt=w&amp;uido=AB9B435AC805DFE93BA349FB5362A08D&amp;ea=1&amp;cs=1_1c3a9137&amp;cb=1636662873443&amp;jobListingId=1007383799744&amp;cpc=42BEC95245890617&amp;jrtk=3-0-1fk8bb2up3of6001-1fk8bb2vdu2f1800-4aeab13752768ad4--6NYlbfkN0AmHEW7ezYoz3qdHICrbgqPAbIqeCN9Klocv_B1s1YAxfzgkXLMblpaM3-0Mjcj2rlRKGXRTDmGVTK4YS3jQ-tBj6VY2UQwcUngeyZs6cGzUTIdmotF-zqe_WrAnUbjwdKNdw7_3fx6mHIIM--0T-EXko5kGKdcPJDLoDFeIE-MNoPfymeU1Y6AiNoUxGPkR3tEglhkaQNt_L5K4S-5mzlNgllFOGScOHslEycwBKCs3cEnTC753Q8hxtSzyHvY8HFwXRQj4JknU_WX6jcRTiGX5GF116ek99GfE0-gjP0vbf6vj2_WEolspzjp1UQl59BxOi5ZwertvV5cRB2lYgMHRwvZmlPKRwe0ndCmkrsten8Jd3-CuxgyN9FjwpRuqSWsQmArIkrDW81Mgo86MibeTtQWUu7sefInV6rPp-0bTEw7wWm8Qxo9RG96kXQ9uQSmk8ne-ifmeOmhwh3fz3xknc1DJyxRg7QGI89HsZyslYUlwwp97jTctfra8Krj590%3D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Required Experience5 years of engineering, electrical engineering preferredBachelors Degree in Elect...</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -538,7 +549,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
         <x:v>3</x:v>
@@ -547,21 +558,21 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:6">
       <x:c r="A5" s="0" t="s">
-        <x:v>0</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="C5" s="0" t="s">
+      <x:c r="D5" s="0" t="s">
         <x:v>15</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>3</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
         <x:v>4</x:v>
@@ -572,19 +583,19 @@
     </x:row>
     <x:row r="6" spans="1:6">
       <x:c r="A6" s="0" t="s">
-        <x:v>0</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="F6" s="0" t="s">
         <x:v>16</x:v>
@@ -592,102 +603,102 @@
     </x:row>
     <x:row r="7" spans="1:6">
       <x:c r="A7" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
       <x:c r="F7" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:6">
       <x:c r="A8" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="D8" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
       <x:c r="E8" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="F8" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:6">
       <x:c r="A9" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
       <x:c r="F9" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:6">
       <x:c r="A10" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
       <x:c r="F10" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:6">
       <x:c r="A11" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="F11" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>